<commit_message>
Adds variable: Alko per 1000
</commit_message>
<xml_diff>
--- a/raw_data/helsinki_demography_subset.xlsx
+++ b/raw_data/helsinki_demography_subset.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kari/Documents/Koulu/ids/mini/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kari/Documents/Koulu/ids/mini/turbine-analysis/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51140346-1D8F-0945-9836-8BC703CC5409}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCD7D77-FD03-8445-AD27-1B5CDF55CF2F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="2700" windowWidth="30480" windowHeight="18160" xr2:uid="{BB512075-5101-8649-AE8C-EB6543C24DA8}"/>
+    <workbookView xWindow="20" yWindow="2700" windowWidth="30480" windowHeight="20160" xr2:uid="{BB512075-5101-8649-AE8C-EB6543C24DA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Alue</t>
   </si>
@@ -159,507 +159,6 @@
     <t>801 Östersundomin peruspiiri</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>Lähde: Helsinki alueittain 2016</t>
-  </si>
-  <si>
-    <t>Käsitemääritelmät ja lähteitä</t>
-  </si>
-  <si>
-    <t>ALUEJAKO</t>
-  </si>
-  <si>
-    <t>Helsingin piirijakojärjestelmä. Hyväksytty kaupunginhallituksessa</t>
-  </si>
-  <si>
-    <t>26.11.2012.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALUESUHDELUKUJA </t>
-  </si>
-  <si>
-    <t>Asukkaita / km2 1.1.2016</t>
-  </si>
-  <si>
-    <t>Työpaikkoja / km2 31.12.2014</t>
-  </si>
-  <si>
-    <t>Kerrosala / ha 31.12.2015</t>
-  </si>
-  <si>
-    <t>ASUMISOLOT 31.12.2015</t>
-  </si>
-  <si>
-    <t>Asuntojen keskikoko on asuinhuoneistojen kokonaisalan ja</t>
-  </si>
-  <si>
-    <t>asuntojen yhteismäärän välinen suhdeluku.</t>
-  </si>
-  <si>
-    <t>Asumisväljyys on asunnon pinta-alan ja siinä asuvien henkilöiden</t>
-  </si>
-  <si>
-    <t>välinen suhde.</t>
-  </si>
-  <si>
-    <t>Asumistiheys on asunnon huoneiden ja siinä asuvien henkilöiden</t>
-  </si>
-  <si>
-    <t>lukumäärän välinen suhde, keittiötä ei ole laskettu</t>
-  </si>
-  <si>
-    <t>huoneeksi.</t>
-  </si>
-  <si>
-    <t>Lähde: Tilastokeskus.</t>
-  </si>
-  <si>
-    <t>ASUNNOT 31.12.2015</t>
-  </si>
-  <si>
-    <t>Huoneistotyypit, keittiö laskettu huoneeksi. Asuntokannan</t>
-  </si>
-  <si>
-    <t>ikä on määritelty rakennuksen käyttöönottovuoden mukaan.</t>
-  </si>
-  <si>
-    <t>ASUNTOKANNAN IKÄ</t>
-  </si>
-  <si>
-    <t>ASUNTOTUOTANTO 1970–2015</t>
-  </si>
-  <si>
-    <t>Lähde: Helsingin kaupungin tietokeskus.</t>
-  </si>
-  <si>
-    <t>HUONEISTOTYYPIT 2015</t>
-  </si>
-  <si>
-    <t>IKÄRAKENNE 1.1.2016</t>
-  </si>
-  <si>
-    <t>Lapset päivähoidon ja peruskoulun ikäryhmityksellä, työikäinen</t>
-  </si>
-  <si>
-    <t>väestö sekä vanhukset omina ryhminään.</t>
-  </si>
-  <si>
-    <t>KOULUT 2016</t>
-  </si>
-  <si>
-    <t>Lähde: Helsingin kaupungin opetusvirasto.</t>
-  </si>
-  <si>
-    <t>KOULUTUSTASO 31.12.2014</t>
-  </si>
-  <si>
-    <t>Väestön koulutusrakennetilastoissa on tiedot 15 vuotta</t>
-  </si>
-  <si>
-    <t>täyttäneen väestön korkeimmasta suorittamasta tutkinnosta</t>
-  </si>
-  <si>
-    <t>ja samantasoisista tutkinnoista viimeksi suoritettu ammatillinen</t>
-  </si>
-  <si>
-    <t>tutkinto.</t>
-  </si>
-  <si>
-    <t>Keskiasteen koulutus sisältää lukiokoulutuksen sekä toisen</t>
-  </si>
-  <si>
-    <t>asteen ammatillinen koulutuksen suorittaneet.</t>
-  </si>
-  <si>
-    <t>Korkea-aste sisältää opistoasteen, ammatillisen korkea-asteen,</t>
-  </si>
-  <si>
-    <t>ammattikorkeakoulun, alemmat korkeakoulututkinnot,</t>
-  </si>
-  <si>
-    <t>ammattikorkeakoulun jatkotutkinnot, ylemmät korkeakoulututkinnot,</t>
-  </si>
-  <si>
-    <t>lääkäreiden erikoistumiskoulutuksen sekä</t>
-  </si>
-  <si>
-    <t>lisensiaatin ja tohtorin tutkinnot.</t>
-  </si>
-  <si>
-    <t>EDUSKUNTAVAALIT 2015</t>
-  </si>
-  <si>
-    <t>Eduskuntavaaleissa vaalipäivänä annettujen äänien osuudet</t>
-  </si>
-  <si>
-    <t>puolueittain.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LASTEN PÄIVÄHOITO 2014 </t>
-  </si>
-  <si>
-    <t>Kaupungin omistamat päiväkodit, yksityiset ostopalvelupäiväkodit</t>
-  </si>
-  <si>
-    <t>ja kunnallinen perhepäivähoito. Kotihoidontukea</t>
-  </si>
-  <si>
-    <t>saavien lasten lukumäärä ja yksityisen hoidon tukea saavien</t>
-  </si>
-  <si>
-    <t>lasten lukumäärä.</t>
-  </si>
-  <si>
-    <t>Lähde: Helsingin kaupungin varhaiskasvatusvirasto.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIIKENNE 2010-2014 </t>
-  </si>
-  <si>
-    <t>Lähde: Helsingin kaupungin kaupunkisuunnitteluvirasto,</t>
-  </si>
-  <si>
-    <t>liikenneonnettomuusrekisteri.</t>
-  </si>
-  <si>
-    <t>Autottomat asuntokunnat (31.12.2013): tieto kuvaa autottomien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asuntokuntien osuutta kaikista asuntokunnista. </t>
-  </si>
-  <si>
-    <t>Lähde: Tilastokeskus ja Suomen ympäristökeskus.</t>
-  </si>
-  <si>
-    <t>PALVELUPISTEET 2016</t>
-  </si>
-  <si>
-    <t>Uimahallit: julkisessa käytössä olevat.</t>
-  </si>
-  <si>
-    <t>Liikuntasalit ja -hallit (sisäliikuntapaikat): liikuntasali,</t>
-  </si>
-  <si>
-    <t>liikuntapaikkojen tyyppikoodi 2150, on muun rakennuksen</t>
-  </si>
-  <si>
-    <t>yhteydessä oleva liikuntatila. Liikuntahalli, liikuntapaikkojen</t>
-  </si>
-  <si>
-    <t>tyyppikoodi 2210, on useiden lajien liikuntatiloja sisältävä</t>
-  </si>
-  <si>
-    <t>rakennus.</t>
-  </si>
-  <si>
-    <t>Pallokenttä (ulkoliikunta): palloiluun, liikuntapaikkojen tyyppikoodi</t>
-  </si>
-  <si>
-    <t>1340, tarkoitettu kenttä. Yksi tai useampi palloilulaji</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mahdollista. </t>
-  </si>
-  <si>
-    <t>Kirkot: Helsingin seurakuntayhtymän hallinnoimat, ortodoksiset</t>
-  </si>
-  <si>
-    <t>ja muut.</t>
-  </si>
-  <si>
-    <t>Päivittäistavarakauppa sisältää elintarvikkeiden, juomien</t>
-  </si>
-  <si>
-    <t>ja tupakan erikoismyymälät sekä laajan tavaravalikoiman</t>
-  </si>
-  <si>
-    <t>vähittäiskaupat, jossa elintarvikkeiden, juomien ja tupakan</t>
-  </si>
-  <si>
-    <t>osuus kokonaismyynnistä on vähintään puolet. Toimialaluokituksen</t>
-  </si>
-  <si>
-    <t>(TOL 2008) toimialat 4711 ja 472.</t>
-  </si>
-  <si>
-    <t>Muut vähittäiskaupat: Toimialaluokituksen (TOL 2008) toimialat 4719, 473-479.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ravintolat: Toimialaluokituksen (TOL 2008) toimiala 561. </t>
-  </si>
-  <si>
-    <t>Kahvilat ja baarit: Toimialaluokituksen (TOL 2008) toimiala 563.</t>
-  </si>
-  <si>
-    <t>Lähde: Valtakunnallinen liikuntapaikkojen tietojärjestelmä (LIPAS), Helsingin seurakuntayhtymä</t>
-  </si>
-  <si>
-    <t>ja Tilastokeskus, toimipaikkarekisteri.</t>
-  </si>
-  <si>
-    <t>PERHEET JA ASUNTOKUNNAT 1.1.2016</t>
-  </si>
-  <si>
-    <t>Perheen muodostavat:</t>
-  </si>
-  <si>
-    <t>- avio- tai avoliitossa olevat vanhemmat ja heidän naimaton</t>
-  </si>
-  <si>
-    <t>tai naimattomat lapsensa tai jompi kumpi vanhemmista</t>
-  </si>
-  <si>
-    <t>naimattomine lapsineen</t>
-  </si>
-  <si>
-    <t>- avio- tai avopari, jonka luona ei asu vakituisesti lapsia.</t>
-  </si>
-  <si>
-    <t>Perhe koostuu vain yhdessä asuvista henkilöistä. Yksin</t>
-  </si>
-  <si>
-    <t>asuvat eivät kuulu perheväestöön.</t>
-  </si>
-  <si>
-    <t>Asuntokunnan muodostavat kaikki samassa asuinhuoneistossa</t>
-  </si>
-  <si>
-    <t>vakinaisesti asuvat henkilöt.</t>
-  </si>
-  <si>
-    <t>RAKENNUSKANTA 2015</t>
-  </si>
-  <si>
-    <t>Rakennusten kerrosalat käyttötarkoituksen mukaan.</t>
-  </si>
-  <si>
-    <t>Pientalo: erilliset pientalot, rivi- ja ketjutalot</t>
-  </si>
-  <si>
-    <t>Kerrostalo: alle ja yli 4 kerrokselliset kerrostalot</t>
-  </si>
-  <si>
-    <t>Liike: liike- ja toimistorakennukset</t>
-  </si>
-  <si>
-    <t>Julkinen: hoitoalan, kokoontumis- ja opetusrakennukset</t>
-  </si>
-  <si>
-    <t>Teollisuus: liikenteen, teollisuus- ja varastorakennukset</t>
-  </si>
-  <si>
-    <t>SOSIAALIPALVELUT 2015</t>
-  </si>
-  <si>
-    <t>1.4.2016 voimaan astunut lakimuutos muutti lastensuojelun asiakkuuden määritelmää. Tästä johtuen asiakasmäärä on vähentynyt.</t>
-  </si>
-  <si>
-    <t>Lähde: Helsingin kaupungin sosiaali- ja terveysvirasto.</t>
-  </si>
-  <si>
-    <t>TERVEYSPALVELUT 2015</t>
-  </si>
-  <si>
-    <t>Avohoitokäynnit: Perusterveydenhuolto (lääkärinvastaanotto,</t>
-  </si>
-  <si>
-    <t>terveyskeskuspäivystys, kotisairaanhoito, hammashuolto</t>
-  </si>
-  <si>
-    <t>ja muu perusterveydenhuolto) ja erikoissairaanhoito</t>
-  </si>
-  <si>
-    <t>(somaattinen ja psykiatrinen erikoissairaanhoito).</t>
-  </si>
-  <si>
-    <t>TOIMITILARAKENNUKSET 31.12.2015</t>
-  </si>
-  <si>
-    <t>Toimitilarakennuksilla tarkoitetaan muita kuin asuinrakennuksia.</t>
-  </si>
-  <si>
-    <t>Toimistot sisältyvät liikerakennuksiin.</t>
-  </si>
-  <si>
-    <t>TULOTASO 2014</t>
-  </si>
-  <si>
-    <t>Tuloilla tarkoitetaan valtionveronalaisia tuloja.</t>
-  </si>
-  <si>
-    <t>Pienituloisia ovat asuntokunnat, joiden käytettävissä oleva rahatulo kulutusyksikköä kohden jää pienemmäksi kuin 60 % koko maan kaikkien kotitalouksien mediaanitulosta.</t>
-  </si>
-  <si>
-    <t>TYÖPAIKAT 31.12.2014</t>
-  </si>
-  <si>
-    <t>Työpaikat on ryhmitelty toimialarakenteen (Toimialaluokitus</t>
-  </si>
-  <si>
-    <t>TOL 2008) mukaan viiteen luokkaan.</t>
-  </si>
-  <si>
-    <t>Tuotanto sisältää toimialat B–F (kaivostoiminta, teollisuus,</t>
-  </si>
-  <si>
-    <t>energia- ja vesihuolto sekä rakentaminen).</t>
-  </si>
-  <si>
-    <t>Kauppa sisältää toimialat G ja I (kauppa sekä majoitus- ja</t>
-  </si>
-  <si>
-    <t>ravitsemistoiminta).</t>
-  </si>
-  <si>
-    <t>Liikenne sisältää toimialan H (kuljetus ja varastointi)</t>
-  </si>
-  <si>
-    <t>Yrityspalvelut sisältää toimialat J–N (informaatio ja</t>
-  </si>
-  <si>
-    <t>viestintä, rahoitus- ja vakuutustoiminta, kiinteistöala sekä</t>
-  </si>
-  <si>
-    <t>ammatillinen, tieteellinen ja tekninen toiminta ja hallinto- ja</t>
-  </si>
-  <si>
-    <t>tukipalvelutoiminta).</t>
-  </si>
-  <si>
-    <t>Yhteiskunnalliset palvelut sisältää toimialat O–U (julkinen</t>
-  </si>
-  <si>
-    <t>hallinto ja maanpuolustus; pakollinen sosiaalivakuutus,</t>
-  </si>
-  <si>
-    <t>koulutus, terveys- ja sosiaalipalvelut, taiteet, viihde ja virkistys,</t>
-  </si>
-  <si>
-    <t>muu palvelutoiminta, kotitaloudet työnantajina sekä</t>
-  </si>
-  <si>
-    <t>kansainvälisten organisaatioiden toiminta).</t>
-  </si>
-  <si>
-    <t>Työpaikat yhteensä sisältää edelliset työpaikkaluokat</t>
-  </si>
-  <si>
-    <t>lisättynä toimialalla A (maa-, metsä ja kalatalous) + X</t>
-  </si>
-  <si>
-    <t>(tuntematon).</t>
-  </si>
-  <si>
-    <t>TYÖVOIMA 2015</t>
-  </si>
-  <si>
-    <t>Työvoimaan luetaan kaikki 15–74-vuotiaat henkilöt, jotka</t>
-  </si>
-  <si>
-    <t>laskentaviikolla olivat työllisiä tai työttömiä.</t>
-  </si>
-  <si>
-    <t>Työlliseen työvoimaan luetaan kaikki 18–74-vuotiaat henkilöt,</t>
-  </si>
-  <si>
-    <t>jotka laskentaviikolla olivat työllisiä.</t>
-  </si>
-  <si>
-    <t>Työttömiin (työtön työvoima) luetaan vuoden 2014 joulukuussa</t>
-  </si>
-  <si>
-    <t>työttömänä olleet 15–74-vuotiaat henkilöt.</t>
-  </si>
-  <si>
-    <t>Nuorisotyöttömyys: 15–24-vuotiaat.</t>
-  </si>
-  <si>
-    <t>Pitkäaikaistyöttömyys: yli vuoden työttömänä yhteisjaksoisesti.</t>
-  </si>
-  <si>
-    <t>Pitkäaikaistyöttömien osuus kaikista työttömistä.</t>
-  </si>
-  <si>
-    <t>Työllisyysaste: Työllisten osuus 20–64-vuotiaasta väestöstä.</t>
-  </si>
-  <si>
-    <t>Lähde: Tilastokeskus, työssäkäyntitilasto ja työ- ja elinkeinoministeriö.</t>
-  </si>
-  <si>
-    <t>ULKOILU 2016</t>
-  </si>
-  <si>
-    <t>Metsäpinta-ala: yleisten alueiden rekisteri, 27.9.2016,</t>
-  </si>
-  <si>
-    <t>hoitoluokat C1–C5.</t>
-  </si>
-  <si>
-    <t>Puistopinta-ala: yleisten alueiden rekisteri, 27.9.2016,</t>
-  </si>
-  <si>
-    <t>hoitoluokat A1–A3 ja B1–B5.</t>
-  </si>
-  <si>
-    <t>Lähde: Helsingin kaupungin rakennusvirasto.</t>
-  </si>
-  <si>
-    <t>Uimarannat: Kunnan terveydensuojeluviranomaisen laatima</t>
-  </si>
-  <si>
-    <t>uimarantaluettelo, suuret ja pienet yleiset uimarannat.</t>
-  </si>
-  <si>
-    <t>Sosiaali- ja terveysministeriön asetus yleisten uimarantojen</t>
-  </si>
-  <si>
-    <t>uimaveden laatuvaatimuksista ja valvonnasta (177/2008).</t>
-  </si>
-  <si>
-    <t>Lähde: Helsingin kaupungin ympäristökeskus.</t>
-  </si>
-  <si>
-    <t>VÄESTÖ 1.1.1986–2026</t>
-  </si>
-  <si>
-    <t>1986–2016 Helsingin väestötilasto, 2017–2026 Helsingin</t>
-  </si>
-  <si>
-    <t>väestöennuste</t>
-  </si>
-  <si>
-    <t>Lähde: Tilastokeskus ja Helsingin kaupungin tietokeskus.</t>
-  </si>
-  <si>
-    <t>VÄESTÖENNUSTE 2026</t>
-  </si>
-  <si>
-    <t>VÄESTÖNMUUTOKSET 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Helsingin muuttoliike kuvaa kaupungin rajat ylittäviä muuttoja. </t>
-  </si>
-  <si>
-    <t>Suur- ja peruspiirien muuttoliike kuvaa kaupungin sisäistä muuttoliikettä alueelta toiselle.</t>
-  </si>
-  <si>
-    <t>ÄIDINKIELI JA KANSALAISUUS 1.1.2016</t>
-  </si>
-  <si>
-    <t>Vieraskieliset = muut kuin suomen-, ruotsin- ja saamenkieliset</t>
-  </si>
-  <si>
-    <t>Alueen kolme yleisintä vierasta kieltä ja niiden osuus kaikista vieraskielisistä.</t>
-  </si>
-  <si>
-    <t>Ulkomaalaistaustaiset = ulkomaan kansalaiset ja ulkomailla</t>
-  </si>
-  <si>
-    <t>syntyneet Suomen kansalaiset</t>
-  </si>
-  <si>
     <t>Suomenkieliset %</t>
   </si>
   <si>
@@ -760,6 +259,12 @@
   </si>
   <si>
     <t>Childern in child-care allowance</t>
+  </si>
+  <si>
+    <t>Alko</t>
+  </si>
+  <si>
+    <t>Alko per 1000</t>
   </si>
 </sst>
 </file>
@@ -770,7 +275,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -943,7 +448,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1266,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA14042-DCA2-A541-BC94-C29708C034E2}">
-  <dimension ref="A1:U258"/>
+  <dimension ref="A1:V258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1282,125 +787,132 @@
     <col min="6" max="11" width="13.83203125" style="11" customWidth="1"/>
     <col min="13" max="13" width="13.83203125" style="11" customWidth="1"/>
     <col min="14" max="14" width="10.83203125" style="11"/>
-    <col min="15" max="21" width="9.1640625" style="7"/>
+    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="22" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>211</v>
+        <v>44</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>212</v>
+        <v>45</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>213</v>
+        <v>46</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>214</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>215</v>
+        <v>48</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>216</v>
+        <v>49</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>217</v>
+        <v>50</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>218</v>
+        <v>51</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>219</v>
+        <v>52</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>220</v>
+        <v>53</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>221</v>
+        <v>54</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>222</v>
+        <v>55</v>
       </c>
       <c r="N1" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="O1" s="28"/>
+        <v>56</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>78</v>
+      </c>
       <c r="P1" s="28"/>
       <c r="Q1" s="28"/>
       <c r="R1" s="28"/>
       <c r="S1" s="28"/>
       <c r="T1" s="28"/>
-    </row>
-    <row r="2" spans="1:21" ht="17" thickBot="1">
+      <c r="U1" s="28"/>
+    </row>
+    <row r="2" spans="1:22" ht="17" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>241</v>
+        <v>74</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>231</v>
+        <v>64</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>232</v>
+        <v>65</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>233</v>
+        <v>66</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>234</v>
+        <v>67</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>235</v>
+        <v>68</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>236</v>
+        <v>69</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>238</v>
+        <v>71</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>239</v>
+        <v>72</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>240</v>
+        <v>73</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>237</v>
+        <v>70</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>244</v>
+        <v>77</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>242</v>
+        <v>75</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="O2" s="29" t="s">
-        <v>224</v>
+        <v>76</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="P2" s="29" t="s">
-        <v>225</v>
+        <v>57</v>
       </c>
       <c r="Q2" s="29" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
       <c r="R2" s="29" t="s">
-        <v>227</v>
+        <v>59</v>
       </c>
       <c r="S2" s="29" t="s">
-        <v>228</v>
+        <v>60</v>
       </c>
       <c r="T2" s="29" t="s">
-        <v>229</v>
-      </c>
-      <c r="U2" s="30" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="17" thickTop="1">
+        <v>61</v>
+      </c>
+      <c r="U2" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="V2" s="30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="17" thickTop="1">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1443,29 +955,32 @@
       <c r="N3" s="15">
         <v>53.338337221014221</v>
       </c>
-      <c r="O3" s="18">
+      <c r="O3">
+        <v>5.730586E-2</v>
+      </c>
+      <c r="P3" s="18">
         <v>15.53</v>
       </c>
-      <c r="P3" s="18">
+      <c r="Q3" s="18">
         <v>25.95</v>
       </c>
-      <c r="Q3" s="18">
+      <c r="R3" s="18">
         <v>18.84</v>
       </c>
-      <c r="R3" s="18">
+      <c r="S3" s="18">
         <v>6.85</v>
       </c>
-      <c r="S3" s="18">
+      <c r="T3" s="18">
         <v>9.85</v>
       </c>
-      <c r="T3" s="18">
+      <c r="U3" s="18">
         <v>11.28</v>
       </c>
-      <c r="U3" s="19">
+      <c r="V3" s="19">
         <v>11.700000000000017</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:22">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1508,29 +1023,32 @@
       <c r="N4" s="16">
         <v>56.290659754160046</v>
       </c>
-      <c r="O4" s="18">
+      <c r="O4">
+        <v>0.13621009000000001</v>
+      </c>
+      <c r="P4" s="18">
         <v>8.42</v>
       </c>
-      <c r="P4" s="18">
+      <c r="Q4" s="18">
         <v>37.78</v>
       </c>
-      <c r="Q4" s="18">
+      <c r="R4" s="18">
         <v>20.7</v>
       </c>
-      <c r="R4" s="18">
+      <c r="S4" s="18">
         <v>12.57</v>
       </c>
-      <c r="S4" s="18">
+      <c r="T4" s="18">
         <v>6.68</v>
       </c>
-      <c r="T4" s="18">
+      <c r="U4" s="18">
         <v>5.28</v>
       </c>
-      <c r="U4" s="19">
+      <c r="V4" s="19">
         <v>8.5699999999999932</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:22">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1573,29 +1091,32 @@
       <c r="N5" s="16">
         <v>54.355756602947615</v>
       </c>
-      <c r="O5" s="18">
+      <c r="O5">
+        <v>0.24034609800000001</v>
+      </c>
+      <c r="P5" s="18">
         <v>9.6</v>
       </c>
-      <c r="P5" s="18">
+      <c r="Q5" s="18">
         <v>36.770000000000003</v>
       </c>
-      <c r="Q5" s="18">
+      <c r="R5" s="18">
         <v>21.95</v>
       </c>
-      <c r="R5" s="18">
+      <c r="S5" s="18">
         <v>9.81</v>
       </c>
-      <c r="S5" s="18">
+      <c r="T5" s="18">
         <v>7.93</v>
       </c>
-      <c r="T5" s="18">
+      <c r="U5" s="18">
         <v>5.36</v>
       </c>
-      <c r="U5" s="19">
+      <c r="V5" s="19">
         <v>8.5799999999999983</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:22">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1638,29 +1159,32 @@
       <c r="N6" s="16">
         <v>56.444218033622008</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6">
+        <v>0.16415644099999999</v>
+      </c>
+      <c r="P6" s="18">
         <v>6.57</v>
       </c>
-      <c r="P6" s="18">
+      <c r="Q6" s="18">
         <v>38.6</v>
       </c>
-      <c r="Q6" s="18">
+      <c r="R6" s="18">
         <v>20.04</v>
       </c>
-      <c r="R6" s="18">
+      <c r="S6" s="18">
         <v>17.489999999999998</v>
       </c>
-      <c r="S6" s="18">
+      <c r="T6" s="18">
         <v>6.5</v>
       </c>
-      <c r="T6" s="18">
+      <c r="U6" s="18">
         <v>3.94</v>
       </c>
-      <c r="U6" s="19">
+      <c r="V6" s="19">
         <v>6.8599999999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:22">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -1703,29 +1227,32 @@
       <c r="N7" s="16">
         <v>60.521831735889243</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7">
+        <v>0.14118710100000001</v>
+      </c>
+      <c r="P7" s="18">
         <v>9.2899999999999991</v>
       </c>
-      <c r="P7" s="18">
+      <c r="Q7" s="18">
         <v>36.840000000000003</v>
       </c>
-      <c r="Q7" s="18">
+      <c r="R7" s="18">
         <v>21.55</v>
       </c>
-      <c r="R7" s="18">
+      <c r="S7" s="18">
         <v>10.08</v>
       </c>
-      <c r="S7" s="18">
+      <c r="T7" s="18">
         <v>7.49</v>
       </c>
-      <c r="T7" s="18">
+      <c r="U7" s="18">
         <v>5.68</v>
       </c>
-      <c r="U7" s="19">
+      <c r="V7" s="19">
         <v>9.0699999999999932</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:22">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1768,29 +1295,32 @@
       <c r="N8" s="16">
         <v>60.062552628413322</v>
       </c>
-      <c r="O8" s="18">
+      <c r="O8">
+        <v>0.13119916000000001</v>
+      </c>
+      <c r="P8" s="18">
         <v>8.57</v>
       </c>
-      <c r="P8" s="18">
+      <c r="Q8" s="18">
         <v>37.17</v>
       </c>
-      <c r="Q8" s="18">
+      <c r="R8" s="18">
         <v>22.62</v>
       </c>
-      <c r="R8" s="18">
+      <c r="S8" s="18">
         <v>10.32</v>
       </c>
-      <c r="S8" s="18">
+      <c r="T8" s="18">
         <v>7.47</v>
       </c>
-      <c r="T8" s="18">
+      <c r="U8" s="18">
         <v>4.9800000000000004</v>
       </c>
-      <c r="U8" s="19">
+      <c r="V8" s="19">
         <v>8.8699999999999903</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:22">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1833,29 +1363,32 @@
       <c r="N9" s="16">
         <v>48.059134456557651</v>
       </c>
-      <c r="O9" s="18">
+      <c r="O9">
+        <v>4.4214529000000002E-2</v>
+      </c>
+      <c r="P9" s="18">
         <v>8.33</v>
       </c>
-      <c r="P9" s="18">
+      <c r="Q9" s="18">
         <v>39.270000000000003</v>
       </c>
-      <c r="Q9" s="18">
+      <c r="R9" s="18">
         <v>18.170000000000002</v>
       </c>
-      <c r="R9" s="18">
+      <c r="S9" s="18">
         <v>14.19</v>
       </c>
-      <c r="S9" s="18">
+      <c r="T9" s="18">
         <v>4.45</v>
       </c>
-      <c r="T9" s="18">
+      <c r="U9" s="18">
         <v>6.18</v>
       </c>
-      <c r="U9" s="19">
+      <c r="V9" s="19">
         <v>9.4099999999999966</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:22">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1898,29 +1431,32 @@
       <c r="N10" s="16">
         <v>54.22789311300528</v>
       </c>
-      <c r="O10" s="18">
+      <c r="O10">
+        <v>4.6691879999999998E-2</v>
+      </c>
+      <c r="P10" s="18">
         <v>14.87</v>
       </c>
-      <c r="P10" s="18">
+      <c r="Q10" s="18">
         <v>27.21</v>
       </c>
-      <c r="Q10" s="18">
+      <c r="R10" s="18">
         <v>18.64</v>
       </c>
-      <c r="R10" s="18">
+      <c r="S10" s="18">
         <v>7.05</v>
       </c>
-      <c r="S10" s="18">
+      <c r="T10" s="18">
         <v>8.11</v>
       </c>
-      <c r="T10" s="18">
+      <c r="U10" s="18">
         <v>11.07</v>
       </c>
-      <c r="U10" s="19">
+      <c r="V10" s="19">
         <v>13.050000000000011</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:22">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1963,29 +1499,32 @@
       <c r="N11" s="16">
         <v>61.190944881889763</v>
       </c>
-      <c r="O11" s="18">
+      <c r="O11">
+        <v>5.7454753999999997E-2</v>
+      </c>
+      <c r="P11" s="18">
         <v>12.830841121495329</v>
       </c>
-      <c r="P11" s="18">
+      <c r="Q11" s="18">
         <v>27.378504672897197</v>
       </c>
-      <c r="Q11" s="18">
+      <c r="R11" s="18">
         <v>22.935514018691588</v>
       </c>
-      <c r="R11" s="18">
+      <c r="S11" s="18">
         <v>7.9186915887850455</v>
       </c>
-      <c r="S11" s="18">
+      <c r="T11" s="18">
         <v>9.9523364485981318</v>
       </c>
-      <c r="T11" s="18">
+      <c r="U11" s="18">
         <v>7.7186915887850471</v>
       </c>
-      <c r="U11" s="19">
+      <c r="V11" s="19">
         <v>11.3</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:22">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
@@ -2028,29 +1567,32 @@
       <c r="N12" s="16">
         <v>50.296989831873553</v>
       </c>
-      <c r="O12" s="18">
+      <c r="O12">
+        <v>5.6724715000000002E-2</v>
+      </c>
+      <c r="P12" s="18">
         <v>9.2100000000000009</v>
       </c>
-      <c r="P12" s="18">
+      <c r="Q12" s="18">
         <v>39.51</v>
       </c>
-      <c r="Q12" s="18">
+      <c r="R12" s="18">
         <v>17.09</v>
       </c>
-      <c r="R12" s="18">
+      <c r="S12" s="18">
         <v>11.87</v>
       </c>
-      <c r="S12" s="18">
+      <c r="T12" s="18">
         <v>5.15</v>
       </c>
-      <c r="T12" s="18">
+      <c r="U12" s="18">
         <v>6.59</v>
       </c>
-      <c r="U12" s="19">
+      <c r="V12" s="19">
         <v>10.579999999999984</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:22">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -2093,29 +1635,32 @@
       <c r="N13" s="16">
         <v>58.658275481736197</v>
       </c>
-      <c r="O13" s="18">
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13" s="18">
         <v>14.753707500834484</v>
       </c>
-      <c r="P13" s="18">
+      <c r="Q13" s="18">
         <v>25.460329570767794</v>
       </c>
-      <c r="Q13" s="18">
+      <c r="R13" s="18">
         <v>20.106677929385476</v>
       </c>
-      <c r="R13" s="18">
+      <c r="S13" s="18">
         <v>6.7555876482489428</v>
       </c>
-      <c r="S13" s="18">
+      <c r="T13" s="18">
         <v>8.5580767999346019</v>
       </c>
-      <c r="T13" s="18">
+      <c r="U13" s="18">
         <v>10.138490568608349</v>
       </c>
-      <c r="U13" s="19">
+      <c r="V13" s="19">
         <v>14.2</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:22">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -2158,29 +1703,32 @@
       <c r="N14" s="16">
         <v>49.403707639626873</v>
       </c>
-      <c r="O14" s="18">
+      <c r="O14">
+        <v>0.111588462</v>
+      </c>
+      <c r="P14" s="18">
         <v>16.68</v>
       </c>
-      <c r="P14" s="18">
+      <c r="Q14" s="18">
         <v>25.71</v>
       </c>
-      <c r="Q14" s="18">
+      <c r="R14" s="18">
         <v>17.64</v>
       </c>
-      <c r="R14" s="18">
+      <c r="S14" s="18">
         <v>4.84</v>
       </c>
-      <c r="S14" s="18">
+      <c r="T14" s="18">
         <v>7.21</v>
       </c>
-      <c r="T14" s="18">
+      <c r="U14" s="18">
         <v>13.62</v>
       </c>
-      <c r="U14" s="19">
+      <c r="V14" s="19">
         <v>14.299999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:22">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -2223,29 +1771,32 @@
       <c r="N15" s="16">
         <v>49.81334926086307</v>
       </c>
-      <c r="O15" s="18">
+      <c r="O15">
+        <v>3.6553716E-2</v>
+      </c>
+      <c r="P15" s="18">
         <v>20.21</v>
       </c>
-      <c r="P15" s="18">
+      <c r="Q15" s="18">
         <v>20.149999999999999</v>
       </c>
-      <c r="Q15" s="18">
+      <c r="R15" s="18">
         <v>15.16</v>
       </c>
-      <c r="R15" s="18">
+      <c r="S15" s="18">
         <v>4.5199999999999996</v>
       </c>
-      <c r="S15" s="18">
+      <c r="T15" s="18">
         <v>9.1300000000000008</v>
       </c>
-      <c r="T15" s="18">
+      <c r="U15" s="18">
         <v>16.45</v>
       </c>
-      <c r="U15" s="19">
+      <c r="V15" s="19">
         <v>14.38000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:22">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
@@ -2288,29 +1839,32 @@
       <c r="N16" s="16">
         <v>67.898637250999798</v>
       </c>
-      <c r="O16" s="18">
+      <c r="O16">
+        <v>5.5104312000000003E-2</v>
+      </c>
+      <c r="P16" s="18">
         <v>14.5</v>
       </c>
-      <c r="P16" s="18">
+      <c r="Q16" s="18">
         <v>17.149999999999999</v>
       </c>
-      <c r="Q16" s="18">
+      <c r="R16" s="18">
         <v>26.86</v>
       </c>
-      <c r="R16" s="18">
+      <c r="S16" s="18">
         <v>4.59</v>
       </c>
-      <c r="S16" s="18">
+      <c r="T16" s="18">
         <v>18.12</v>
       </c>
-      <c r="T16" s="18">
+      <c r="U16" s="18">
         <v>8.5500000000000007</v>
       </c>
-      <c r="U16" s="19">
+      <c r="V16" s="19">
         <v>10.230000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:22">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -2353,29 +1907,32 @@
       <c r="N17" s="16">
         <v>72.185027388922705</v>
       </c>
-      <c r="O17" s="18">
+      <c r="O17">
+        <v>3.4402092000000002E-2</v>
+      </c>
+      <c r="P17" s="18">
         <v>13.05</v>
       </c>
-      <c r="P17" s="18">
+      <c r="Q17" s="18">
         <v>18.55</v>
       </c>
-      <c r="Q17" s="18">
+      <c r="R17" s="18">
         <v>28.59</v>
       </c>
-      <c r="R17" s="18">
+      <c r="S17" s="18">
         <v>4.2300000000000004</v>
       </c>
-      <c r="S17" s="18">
+      <c r="T17" s="18">
         <v>18.149999999999999</v>
       </c>
-      <c r="T17" s="18">
+      <c r="U17" s="18">
         <v>7.46</v>
       </c>
-      <c r="U17" s="19">
+      <c r="V17" s="19">
         <v>9.9700000000000131</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:22">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -2418,29 +1975,32 @@
       <c r="N18" s="16">
         <v>75.460122699386503</v>
       </c>
-      <c r="O18" s="18">
+      <c r="O18">
+        <v>8.3773141999999995E-2</v>
+      </c>
+      <c r="P18" s="18">
         <v>12.96</v>
       </c>
-      <c r="P18" s="18">
+      <c r="Q18" s="18">
         <v>17.09</v>
       </c>
-      <c r="Q18" s="18">
+      <c r="R18" s="18">
         <v>28.55</v>
       </c>
-      <c r="R18" s="18">
+      <c r="S18" s="18">
         <v>4.16</v>
       </c>
-      <c r="S18" s="18">
+      <c r="T18" s="18">
         <v>18.690000000000001</v>
       </c>
-      <c r="T18" s="18">
+      <c r="U18" s="18">
         <v>8.31</v>
       </c>
-      <c r="U18" s="19">
+      <c r="V18" s="19">
         <v>10.239999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:22">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -2483,29 +2043,32 @@
       <c r="N19" s="16">
         <v>68.521155410903177</v>
       </c>
-      <c r="O19" s="18">
+      <c r="O19">
+        <v>6.3893680999999994E-2</v>
+      </c>
+      <c r="P19" s="18">
         <v>17.670000000000002</v>
       </c>
-      <c r="P19" s="18">
+      <c r="Q19" s="18">
         <v>18.37</v>
       </c>
-      <c r="Q19" s="18">
+      <c r="R19" s="18">
         <v>19.71</v>
       </c>
-      <c r="R19" s="18">
+      <c r="S19" s="18">
         <v>4.21</v>
       </c>
-      <c r="S19" s="18">
+      <c r="T19" s="18">
         <v>14.52</v>
       </c>
-      <c r="T19" s="18">
+      <c r="U19" s="18">
         <v>12.06</v>
       </c>
-      <c r="U19" s="19">
+      <c r="V19" s="19">
         <v>13.459999999999994</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:22">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
@@ -2548,29 +2111,32 @@
       <c r="N20" s="16">
         <v>62.838948233360725</v>
       </c>
-      <c r="O20" s="18">
+      <c r="O20">
+        <v>0.108471635</v>
+      </c>
+      <c r="P20" s="18">
         <v>13.85</v>
       </c>
-      <c r="P20" s="18">
+      <c r="Q20" s="18">
         <v>14.55</v>
       </c>
-      <c r="Q20" s="18">
+      <c r="R20" s="18">
         <v>27.42</v>
       </c>
-      <c r="R20" s="18">
+      <c r="S20" s="18">
         <v>5.18</v>
       </c>
-      <c r="S20" s="18">
+      <c r="T20" s="18">
         <v>19.899999999999999</v>
       </c>
-      <c r="T20" s="18">
+      <c r="U20" s="18">
         <v>9.39</v>
       </c>
-      <c r="U20" s="19">
+      <c r="V20" s="19">
         <v>9.7099999999999937</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:22">
       <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
@@ -2613,29 +2179,32 @@
       <c r="N21" s="16">
         <v>57.953503874677118</v>
       </c>
-      <c r="O21" s="18">
-        <v>16.53</v>
+      <c r="O21">
+        <v>4.0222026000000001E-2</v>
       </c>
       <c r="P21" s="18">
         <v>16.53</v>
       </c>
       <c r="Q21" s="18">
+        <v>16.53</v>
+      </c>
+      <c r="R21" s="18">
         <v>25.91</v>
       </c>
-      <c r="R21" s="18">
+      <c r="S21" s="18">
         <v>5.08</v>
       </c>
-      <c r="S21" s="18">
+      <c r="T21" s="18">
         <v>17.93</v>
       </c>
-      <c r="T21" s="18">
+      <c r="U21" s="18">
         <v>8.31</v>
       </c>
-      <c r="U21" s="19">
+      <c r="V21" s="19">
         <v>9.710000000000008</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:22">
       <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
@@ -2678,29 +2247,32 @@
       <c r="N22" s="16">
         <v>38.706498625589958</v>
       </c>
-      <c r="O22" s="18">
+      <c r="O22">
+        <v>4.6813192000000003E-2</v>
+      </c>
+      <c r="P22" s="18">
         <v>16.12</v>
       </c>
-      <c r="P22" s="18">
+      <c r="Q22" s="18">
         <v>31.83</v>
       </c>
-      <c r="Q22" s="18">
+      <c r="R22" s="18">
         <v>15.88</v>
       </c>
-      <c r="R22" s="18">
+      <c r="S22" s="18">
         <v>4.62</v>
       </c>
-      <c r="S22" s="18">
+      <c r="T22" s="18">
         <v>7.68</v>
       </c>
-      <c r="T22" s="18">
+      <c r="U22" s="18">
         <v>11.12</v>
       </c>
-      <c r="U22" s="19">
+      <c r="V22" s="19">
         <v>12.75</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:22">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
@@ -2743,29 +2315,32 @@
       <c r="N23" s="16">
         <v>54.706004570953667</v>
       </c>
-      <c r="O23" s="18">
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23" s="18">
         <v>19.12</v>
       </c>
-      <c r="P23" s="18">
+      <c r="Q23" s="18">
         <v>18.079999999999998</v>
       </c>
-      <c r="Q23" s="18">
+      <c r="R23" s="18">
         <v>18.79</v>
       </c>
-      <c r="R23" s="18">
+      <c r="S23" s="18">
         <v>4.79</v>
       </c>
-      <c r="S23" s="18">
+      <c r="T23" s="18">
         <v>12.5</v>
       </c>
-      <c r="T23" s="18">
+      <c r="U23" s="18">
         <v>13.98</v>
       </c>
-      <c r="U23" s="19">
+      <c r="V23" s="19">
         <v>12.739999999999995</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:22">
       <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
@@ -2808,29 +2383,32 @@
       <c r="N24" s="16">
         <v>21.831561733442356</v>
       </c>
-      <c r="O24" s="18">
+      <c r="O24">
+        <v>0.14216661899999999</v>
+      </c>
+      <c r="P24" s="18">
         <v>12.63</v>
       </c>
-      <c r="P24" s="18">
+      <c r="Q24" s="18">
         <v>45.05</v>
       </c>
-      <c r="Q24" s="18">
+      <c r="R24" s="18">
         <v>13.05</v>
       </c>
-      <c r="R24" s="18">
+      <c r="S24" s="18">
         <v>4.8899999999999997</v>
       </c>
-      <c r="S24" s="18">
+      <c r="T24" s="18">
         <v>4.34</v>
       </c>
-      <c r="T24" s="18">
+      <c r="U24" s="18">
         <v>8.25</v>
       </c>
-      <c r="U24" s="19">
+      <c r="V24" s="19">
         <v>11.789999999999992</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:22">
       <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
@@ -2873,29 +2451,32 @@
       <c r="N25" s="16">
         <v>17.879794623980672</v>
       </c>
-      <c r="O25" s="18">
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25" s="18">
         <v>15.19</v>
       </c>
-      <c r="P25" s="18">
+      <c r="Q25" s="18">
         <v>38.75</v>
       </c>
-      <c r="Q25" s="18">
+      <c r="R25" s="18">
         <v>14.23</v>
       </c>
-      <c r="R25" s="18">
+      <c r="S25" s="18">
         <v>3.84</v>
       </c>
-      <c r="S25" s="18">
+      <c r="T25" s="18">
         <v>5</v>
       </c>
-      <c r="T25" s="18">
+      <c r="U25" s="18">
         <v>10.46</v>
       </c>
-      <c r="U25" s="19">
+      <c r="V25" s="19">
         <v>12.530000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:22">
       <c r="A26" s="4" t="s">
         <v>24</v>
       </c>
@@ -2938,29 +2519,32 @@
       <c r="N26" s="16">
         <v>46.973903387007219</v>
       </c>
-      <c r="O26" s="18">
+      <c r="O26">
+        <v>6.9773931999999997E-2</v>
+      </c>
+      <c r="P26" s="18">
         <v>17.45</v>
       </c>
-      <c r="P26" s="18">
+      <c r="Q26" s="18">
         <v>25.95</v>
       </c>
-      <c r="Q26" s="18">
+      <c r="R26" s="18">
         <v>17.399999999999999</v>
       </c>
-      <c r="R26" s="18">
+      <c r="S26" s="18">
         <v>4.8</v>
       </c>
-      <c r="S26" s="18">
+      <c r="T26" s="18">
         <v>9.26</v>
       </c>
-      <c r="T26" s="18">
+      <c r="U26" s="18">
         <v>11.53</v>
       </c>
-      <c r="U26" s="19">
+      <c r="V26" s="19">
         <v>13.61</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:22">
       <c r="A27" s="4" t="s">
         <v>25</v>
       </c>
@@ -3003,29 +2587,32 @@
       <c r="N27" s="16">
         <v>21.234240212342403</v>
       </c>
-      <c r="O27" s="18">
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27" s="18">
         <v>13.51</v>
       </c>
-      <c r="P27" s="18">
+      <c r="Q27" s="18">
         <v>41.72</v>
       </c>
-      <c r="Q27" s="18">
+      <c r="R27" s="18">
         <v>13.17</v>
       </c>
-      <c r="R27" s="18">
+      <c r="S27" s="18">
         <v>4.96</v>
       </c>
-      <c r="S27" s="18">
+      <c r="T27" s="18">
         <v>4.1100000000000003</v>
       </c>
-      <c r="T27" s="18">
+      <c r="U27" s="18">
         <v>10.55</v>
       </c>
-      <c r="U27" s="19">
+      <c r="V27" s="19">
         <v>11.980000000000018</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:22">
       <c r="A28" s="4" t="s">
         <v>26</v>
       </c>
@@ -3068,29 +2655,32 @@
       <c r="N28" s="16">
         <v>45.04370346390418</v>
       </c>
-      <c r="O28" s="18">
+      <c r="O28">
+        <v>2.0409205E-2</v>
+      </c>
+      <c r="P28" s="18">
         <v>20.39</v>
       </c>
-      <c r="P28" s="18">
+      <c r="Q28" s="18">
         <v>20.62</v>
       </c>
-      <c r="Q28" s="18">
+      <c r="R28" s="18">
         <v>14.67</v>
       </c>
-      <c r="R28" s="18">
+      <c r="S28" s="18">
         <v>3.09</v>
       </c>
-      <c r="S28" s="18">
+      <c r="T28" s="18">
         <v>9.2799999999999994</v>
       </c>
-      <c r="T28" s="18">
+      <c r="U28" s="18">
         <v>17.03</v>
       </c>
-      <c r="U28" s="19">
+      <c r="V28" s="19">
         <v>14.919999999999987</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:22">
       <c r="A29" s="4" t="s">
         <v>27</v>
       </c>
@@ -3133,29 +2723,32 @@
       <c r="N29" s="16">
         <v>51.596058283500376</v>
       </c>
-      <c r="O29" s="18">
+      <c r="O29">
+        <v>4.0696728000000001E-2</v>
+      </c>
+      <c r="P29" s="18">
         <v>18.559999999999999</v>
       </c>
-      <c r="P29" s="18">
+      <c r="Q29" s="18">
         <v>18.079999999999998</v>
       </c>
-      <c r="Q29" s="18">
+      <c r="R29" s="18">
         <v>19.61</v>
       </c>
-      <c r="R29" s="18">
+      <c r="S29" s="18">
         <v>3.2</v>
       </c>
-      <c r="S29" s="18">
+      <c r="T29" s="18">
         <v>11.05</v>
       </c>
-      <c r="T29" s="18">
+      <c r="U29" s="18">
         <v>14.12</v>
       </c>
-      <c r="U29" s="19">
+      <c r="V29" s="19">
         <v>15.379999999999995</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:22">
       <c r="A30" s="4" t="s">
         <v>28</v>
       </c>
@@ -3198,29 +2791,32 @@
       <c r="N30" s="16">
         <v>52.43827790246889</v>
       </c>
-      <c r="O30" s="18">
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30" s="18">
         <v>22.56</v>
       </c>
-      <c r="P30" s="18">
+      <c r="Q30" s="18">
         <v>19.04</v>
       </c>
-      <c r="Q30" s="18">
+      <c r="R30" s="18">
         <v>13.93</v>
       </c>
-      <c r="R30" s="18">
+      <c r="S30" s="18">
         <v>2.9</v>
       </c>
-      <c r="S30" s="18">
+      <c r="T30" s="18">
         <v>8.93</v>
       </c>
-      <c r="T30" s="18">
+      <c r="U30" s="18">
         <v>16.3</v>
       </c>
-      <c r="U30" s="19">
+      <c r="V30" s="19">
         <v>16.340000000000018</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:22">
       <c r="A31" s="4" t="s">
         <v>29</v>
       </c>
@@ -3263,29 +2859,32 @@
       <c r="N31" s="16">
         <v>44.451881600475978</v>
       </c>
-      <c r="O31" s="18">
+      <c r="O31">
+        <v>3.4580538000000001E-2</v>
+      </c>
+      <c r="P31" s="18">
         <v>20.7</v>
       </c>
-      <c r="P31" s="18">
+      <c r="Q31" s="18">
         <v>21.58</v>
       </c>
-      <c r="Q31" s="18">
+      <c r="R31" s="18">
         <v>13.64</v>
       </c>
-      <c r="R31" s="18">
+      <c r="S31" s="18">
         <v>3.54</v>
       </c>
-      <c r="S31" s="18">
+      <c r="T31" s="18">
         <v>8.8699999999999992</v>
       </c>
-      <c r="T31" s="18">
+      <c r="U31" s="18">
         <v>17.2</v>
       </c>
-      <c r="U31" s="19">
+      <c r="V31" s="19">
         <v>14.469999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:22">
       <c r="A32" s="4" t="s">
         <v>30</v>
       </c>
@@ -3328,29 +2927,32 @@
       <c r="N32" s="16">
         <v>32.855387136419502</v>
       </c>
-      <c r="O32" s="18">
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32" s="18">
         <v>21.81</v>
       </c>
-      <c r="P32" s="18">
+      <c r="Q32" s="18">
         <v>21.52</v>
       </c>
-      <c r="Q32" s="18">
+      <c r="R32" s="18">
         <v>12.01</v>
       </c>
-      <c r="R32" s="18">
+      <c r="S32" s="18">
         <v>2.92</v>
       </c>
-      <c r="S32" s="18">
+      <c r="T32" s="18">
         <v>7.57</v>
       </c>
-      <c r="T32" s="18">
+      <c r="U32" s="18">
         <v>19.41</v>
       </c>
-      <c r="U32" s="19">
+      <c r="V32" s="19">
         <v>14.760000000000005</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:22">
       <c r="A33" s="4" t="s">
         <v>31</v>
       </c>
@@ -3393,29 +2995,32 @@
       <c r="N33" s="16">
         <v>35.791915984857738</v>
       </c>
-      <c r="O33" s="18">
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33" s="18">
         <v>19.97</v>
       </c>
-      <c r="P33" s="18">
+      <c r="Q33" s="18">
         <v>24.62</v>
       </c>
-      <c r="Q33" s="18">
+      <c r="R33" s="18">
         <v>12.9</v>
       </c>
-      <c r="R33" s="18">
+      <c r="S33" s="18">
         <v>2.68</v>
       </c>
-      <c r="S33" s="18">
+      <c r="T33" s="18">
         <v>8.51</v>
       </c>
-      <c r="T33" s="18">
+      <c r="U33" s="18">
         <v>16.3</v>
       </c>
-      <c r="U33" s="19">
+      <c r="V33" s="19">
         <v>15.019999999999996</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:22">
       <c r="A34" s="4" t="s">
         <v>32</v>
       </c>
@@ -3458,29 +3063,32 @@
       <c r="N34" s="16">
         <v>54.632063074901453</v>
       </c>
-      <c r="O34" s="18">
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34" s="18">
         <v>25.58</v>
       </c>
-      <c r="P34" s="18">
+      <c r="Q34" s="18">
         <v>9.6999999999999993</v>
       </c>
-      <c r="Q34" s="18">
+      <c r="R34" s="18">
         <v>9.86</v>
       </c>
-      <c r="R34" s="18">
+      <c r="S34" s="18">
         <v>1.79</v>
       </c>
-      <c r="S34" s="18">
+      <c r="T34" s="18">
         <v>10.25</v>
       </c>
-      <c r="T34" s="18">
+      <c r="U34" s="18">
         <v>27.33</v>
       </c>
-      <c r="U34" s="19">
+      <c r="V34" s="19">
         <v>15.490000000000009</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:22">
       <c r="A35" s="4" t="s">
         <v>33</v>
       </c>
@@ -3523,29 +3131,32 @@
       <c r="N35" s="16">
         <v>50.795702399224496</v>
       </c>
-      <c r="O35" s="18">
+      <c r="O35">
+        <v>2.0253165E-2</v>
+      </c>
+      <c r="P35" s="18">
         <v>15.8</v>
       </c>
-      <c r="P35" s="18">
+      <c r="Q35" s="18">
         <v>26.97</v>
       </c>
-      <c r="Q35" s="18">
+      <c r="R35" s="18">
         <v>18.54</v>
       </c>
-      <c r="R35" s="18">
+      <c r="S35" s="18">
         <v>6.35</v>
       </c>
-      <c r="S35" s="18">
+      <c r="T35" s="18">
         <v>10.050000000000001</v>
       </c>
-      <c r="T35" s="18">
+      <c r="U35" s="18">
         <v>11.59</v>
       </c>
-      <c r="U35" s="19">
+      <c r="V35" s="19">
         <v>10.700000000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:21">
+    <row r="36" spans="1:22">
       <c r="A36" s="4" t="s">
         <v>34</v>
       </c>
@@ -3588,29 +3199,32 @@
       <c r="N36" s="16">
         <v>45.981905268759974</v>
       </c>
-      <c r="O36" s="18">
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36" s="18">
         <v>7.36</v>
       </c>
-      <c r="P36" s="18">
+      <c r="Q36" s="18">
         <v>40.64</v>
       </c>
-      <c r="Q36" s="18">
+      <c r="R36" s="18">
         <v>16.68</v>
       </c>
-      <c r="R36" s="18">
+      <c r="S36" s="18">
         <v>17.18</v>
       </c>
-      <c r="S36" s="18">
+      <c r="T36" s="18">
         <v>4.74</v>
       </c>
-      <c r="T36" s="18">
+      <c r="U36" s="18">
         <v>5.7</v>
       </c>
-      <c r="U36" s="19">
+      <c r="V36" s="19">
         <v>7.6999999999999886</v>
       </c>
     </row>
-    <row r="37" spans="1:21">
+    <row r="37" spans="1:22">
       <c r="A37" s="4" t="s">
         <v>35</v>
       </c>
@@ -3653,29 +3267,32 @@
       <c r="N37" s="16">
         <v>56.473184432258925</v>
       </c>
-      <c r="O37" s="18">
+      <c r="O37">
+        <v>3.5133330999999997E-2</v>
+      </c>
+      <c r="P37" s="18">
         <v>17.693939639028699</v>
       </c>
-      <c r="P37" s="18">
+      <c r="Q37" s="18">
         <v>21.05354843124934</v>
       </c>
-      <c r="Q37" s="18">
+      <c r="R37" s="18">
         <v>21.270678703191006</v>
       </c>
-      <c r="R37" s="18">
+      <c r="S37" s="18">
         <v>4.4197520110991517</v>
       </c>
-      <c r="S37" s="18">
+      <c r="T37" s="18">
         <v>12.523252847890603</v>
       </c>
-      <c r="T37" s="18">
+      <c r="U37" s="18">
         <v>12.633373358302277</v>
       </c>
-      <c r="U37" s="19">
+      <c r="V37" s="19">
         <v>10.4</v>
       </c>
     </row>
-    <row r="38" spans="1:21">
+    <row r="38" spans="1:22">
       <c r="A38" s="4" t="s">
         <v>36</v>
       </c>
@@ -3718,29 +3335,32 @@
       <c r="N38" s="16">
         <v>41.223974763406943</v>
       </c>
-      <c r="O38" s="18">
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38" s="18">
         <v>14.89</v>
       </c>
-      <c r="P38" s="18">
+      <c r="Q38" s="18">
         <v>33.049999999999997</v>
       </c>
-      <c r="Q38" s="18">
+      <c r="R38" s="18">
         <v>14.51</v>
       </c>
-      <c r="R38" s="18">
+      <c r="S38" s="18">
         <v>6.79</v>
       </c>
-      <c r="S38" s="18">
+      <c r="T38" s="18">
         <v>7.37</v>
       </c>
-      <c r="T38" s="18">
+      <c r="U38" s="18">
         <v>11.44</v>
       </c>
-      <c r="U38" s="19">
+      <c r="V38" s="19">
         <v>11.950000000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:21">
+    <row r="39" spans="1:22">
       <c r="A39" s="4" t="s">
         <v>37</v>
       </c>
@@ -3783,29 +3403,32 @@
       <c r="N39" s="16">
         <v>50.503537868293961</v>
       </c>
-      <c r="O39" s="18">
+      <c r="O39">
+        <v>5.4834582E-2</v>
+      </c>
+      <c r="P39" s="18">
         <v>23.15</v>
       </c>
-      <c r="P39" s="18">
+      <c r="Q39" s="18">
         <v>19.579999999999998</v>
       </c>
-      <c r="Q39" s="18">
+      <c r="R39" s="18">
         <v>12.97</v>
       </c>
-      <c r="R39" s="18">
+      <c r="S39" s="18">
         <v>4.7699999999999996</v>
       </c>
-      <c r="S39" s="18">
+      <c r="T39" s="18">
         <v>9.0500000000000007</v>
       </c>
-      <c r="T39" s="18">
+      <c r="U39" s="18">
         <v>17.75</v>
       </c>
-      <c r="U39" s="19">
+      <c r="V39" s="19">
         <v>12.730000000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:21">
+    <row r="40" spans="1:22">
       <c r="A40" s="4" t="s">
         <v>38</v>
       </c>
@@ -3848,29 +3471,32 @@
       <c r="N40" s="16">
         <v>50.119573215599708</v>
       </c>
-      <c r="O40" s="18">
+      <c r="O40">
+        <v>0.13492241999999999</v>
+      </c>
+      <c r="P40" s="18">
         <v>20.18</v>
       </c>
-      <c r="P40" s="18">
+      <c r="Q40" s="18">
         <v>25.1</v>
       </c>
-      <c r="Q40" s="18">
+      <c r="R40" s="18">
         <v>14.07</v>
       </c>
-      <c r="R40" s="18">
+      <c r="S40" s="18">
         <v>5.49</v>
       </c>
-      <c r="S40" s="18">
+      <c r="T40" s="18">
         <v>8.33</v>
       </c>
-      <c r="T40" s="18">
+      <c r="U40" s="18">
         <v>15.3</v>
       </c>
-      <c r="U40" s="19">
+      <c r="V40" s="19">
         <v>11.530000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:21">
+    <row r="41" spans="1:22">
       <c r="A41" s="4" t="s">
         <v>39</v>
       </c>
@@ -3913,29 +3539,32 @@
       <c r="N41" s="16">
         <v>50.657894736842103</v>
       </c>
-      <c r="O41" s="18">
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41" s="18">
         <v>27.173000000000002</v>
       </c>
-      <c r="P41" s="18">
+      <c r="Q41" s="18">
         <v>18.757000000000001</v>
       </c>
-      <c r="Q41" s="18">
+      <c r="R41" s="18">
         <v>15.262</v>
       </c>
-      <c r="R41" s="18">
+      <c r="S41" s="18">
         <v>4.62</v>
       </c>
-      <c r="S41" s="18">
+      <c r="T41" s="18">
         <v>10.790000000000001</v>
       </c>
-      <c r="T41" s="18">
+      <c r="U41" s="18">
         <v>19.186999999999998</v>
       </c>
-      <c r="U41" s="19">
+      <c r="V41" s="19">
         <v>4.2109999999999843</v>
       </c>
     </row>
-    <row r="42" spans="1:21">
+    <row r="42" spans="1:22">
       <c r="A42" s="4" t="s">
         <v>40</v>
       </c>
@@ -3978,29 +3607,32 @@
       <c r="N42" s="16">
         <v>50.95445501962682</v>
       </c>
-      <c r="O42" s="18">
+      <c r="O42">
+        <v>5.3191489000000002E-2</v>
+      </c>
+      <c r="P42" s="18">
         <v>26.68</v>
       </c>
-      <c r="P42" s="18">
+      <c r="Q42" s="18">
         <v>14</v>
       </c>
-      <c r="Q42" s="18">
+      <c r="R42" s="18">
         <v>10.71</v>
       </c>
-      <c r="R42" s="18">
+      <c r="S42" s="18">
         <v>3.51</v>
       </c>
-      <c r="S42" s="18">
+      <c r="T42" s="18">
         <v>10.199999999999999</v>
       </c>
-      <c r="T42" s="18">
+      <c r="U42" s="18">
         <v>21.43</v>
       </c>
-      <c r="U42" s="19">
+      <c r="V42" s="19">
         <v>13.469999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:21">
+    <row r="43" spans="1:22">
       <c r="A43" s="4" t="s">
         <v>41</v>
       </c>
@@ -4043,29 +3675,32 @@
       <c r="N43" s="16">
         <v>50.226417153145285</v>
       </c>
-      <c r="O43" s="18">
+      <c r="O43">
+        <v>2.6426363000000001E-2</v>
+      </c>
+      <c r="P43" s="18">
         <v>21.32</v>
       </c>
-      <c r="P43" s="18">
+      <c r="Q43" s="18">
         <v>21.79</v>
       </c>
-      <c r="Q43" s="18">
+      <c r="R43" s="18">
         <v>14.18</v>
       </c>
-      <c r="R43" s="18">
+      <c r="S43" s="18">
         <v>5.58</v>
       </c>
-      <c r="S43" s="18">
+      <c r="T43" s="18">
         <v>8.39</v>
       </c>
-      <c r="T43" s="18">
+      <c r="U43" s="18">
         <v>16.05</v>
       </c>
-      <c r="U43" s="19">
+      <c r="V43" s="19">
         <v>12.690000000000012</v>
       </c>
     </row>
-    <row r="44" spans="1:21">
+    <row r="44" spans="1:22">
       <c r="A44" s="4" t="s">
         <v>42</v>
       </c>
@@ -4108,29 +3743,32 @@
       <c r="N44" s="16">
         <v>10.45016077170418</v>
       </c>
-      <c r="O44" s="18">
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44" s="18">
         <v>6.61</v>
       </c>
-      <c r="P44" s="18">
+      <c r="Q44" s="18">
         <v>40.04</v>
       </c>
-      <c r="Q44" s="18">
+      <c r="R44" s="18">
         <v>7.97</v>
       </c>
-      <c r="R44" s="18">
+      <c r="S44" s="18">
         <v>20.65</v>
       </c>
-      <c r="S44" s="18">
+      <c r="T44" s="18">
         <v>2.08</v>
       </c>
-      <c r="T44" s="18">
+      <c r="U44" s="18">
         <v>9.8699999999999992</v>
       </c>
-      <c r="U44" s="19">
+      <c r="V44" s="19">
         <v>12.780000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:21">
+    <row r="45" spans="1:22">
       <c r="A45" s="4" t="s">
         <v>43</v>
       </c>
@@ -4173,32 +3811,33 @@
       <c r="N45" s="16">
         <v>10.45016077170418</v>
       </c>
-      <c r="O45" s="18">
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45" s="18">
         <v>6.61</v>
       </c>
-      <c r="P45" s="18">
+      <c r="Q45" s="18">
         <v>40.04</v>
       </c>
-      <c r="Q45" s="18">
+      <c r="R45" s="18">
         <v>7.97</v>
       </c>
-      <c r="R45" s="18">
+      <c r="S45" s="18">
         <v>20.65</v>
       </c>
-      <c r="S45" s="18">
+      <c r="T45" s="18">
         <v>2.08</v>
       </c>
-      <c r="T45" s="18">
+      <c r="U45" s="18">
         <v>9.8699999999999992</v>
       </c>
-      <c r="U45" s="19">
+      <c r="V45" s="19">
         <v>12.780000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:21">
-      <c r="A46" s="4" t="s">
-        <v>44</v>
-      </c>
+    <row r="46" spans="1:22">
+      <c r="A46" s="4"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -4212,30 +3851,24 @@
       <c r="L46" s="7"/>
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
-      <c r="O46" s="19"/>
       <c r="P46" s="19"/>
       <c r="Q46" s="19"/>
       <c r="R46" s="19"/>
       <c r="S46" s="19"/>
       <c r="T46" s="19"/>
       <c r="U46" s="19"/>
-    </row>
-    <row r="47" spans="1:21">
-      <c r="A47" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="V46" s="19"/>
+    </row>
+    <row r="47" spans="1:22">
+      <c r="A47" s="4"/>
       <c r="L47" s="25"/>
     </row>
-    <row r="48" spans="1:21">
-      <c r="A48" s="4" t="s">
-        <v>44</v>
-      </c>
+    <row r="48" spans="1:22">
+      <c r="A48" s="4"/>
       <c r="L48" s="25"/>
     </row>
     <row r="49" spans="1:12">
-      <c r="A49" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="A49" s="5"/>
       <c r="L49" s="25"/>
     </row>
     <row r="50" spans="1:12">
@@ -4243,1170 +3876,627 @@
       <c r="L50" s="25"/>
     </row>
     <row r="51" spans="1:12">
-      <c r="A51" s="7" t="s">
-        <v>47</v>
-      </c>
       <c r="L51" s="25"/>
     </row>
     <row r="52" spans="1:12">
-      <c r="A52" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="L52" s="25"/>
     </row>
     <row r="53" spans="1:12">
-      <c r="A53" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="L53" s="25"/>
     </row>
     <row r="54" spans="1:12">
       <c r="L54" s="25"/>
     </row>
     <row r="55" spans="1:12">
-      <c r="A55" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="L55" s="25"/>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="7" t="s">
-        <v>51</v>
-      </c>
       <c r="L56" s="25"/>
     </row>
     <row r="57" spans="1:12">
-      <c r="A57" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="L57" s="25"/>
     </row>
     <row r="58" spans="1:12">
-      <c r="A58" s="7" t="s">
-        <v>53</v>
-      </c>
       <c r="L58" s="25"/>
     </row>
     <row r="59" spans="1:12">
       <c r="L59" s="25"/>
     </row>
     <row r="60" spans="1:12">
-      <c r="A60" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="L60" s="25"/>
     </row>
     <row r="61" spans="1:12">
-      <c r="A61" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="L61" s="25"/>
     </row>
     <row r="62" spans="1:12">
-      <c r="A62" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="L62" s="25"/>
     </row>
     <row r="63" spans="1:12">
-      <c r="A63" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="L63" s="25"/>
     </row>
     <row r="64" spans="1:12">
-      <c r="A64" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="L64" s="25"/>
     </row>
-    <row r="65" spans="1:12">
-      <c r="A65" s="7" t="s">
-        <v>59</v>
-      </c>
+    <row r="65" spans="12:12">
       <c r="L65" s="25"/>
     </row>
-    <row r="66" spans="1:12">
-      <c r="A66" s="7" t="s">
-        <v>60</v>
-      </c>
+    <row r="66" spans="12:12">
       <c r="L66" s="25"/>
     </row>
-    <row r="67" spans="1:12">
-      <c r="A67" s="7" t="s">
-        <v>61</v>
-      </c>
+    <row r="67" spans="12:12">
       <c r="L67" s="25"/>
     </row>
-    <row r="68" spans="1:12">
-      <c r="A68" s="7" t="s">
-        <v>62</v>
-      </c>
+    <row r="68" spans="12:12">
       <c r="L68" s="25"/>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="12:12">
       <c r="L69" s="25"/>
     </row>
-    <row r="70" spans="1:12">
-      <c r="A70" s="7" t="s">
-        <v>63</v>
-      </c>
+    <row r="70" spans="12:12">
       <c r="L70" s="25"/>
     </row>
-    <row r="71" spans="1:12">
-      <c r="A71" s="7" t="s">
-        <v>64</v>
-      </c>
+    <row r="71" spans="12:12">
       <c r="L71" s="25"/>
     </row>
-    <row r="72" spans="1:12">
-      <c r="A72" s="7" t="s">
-        <v>65</v>
-      </c>
+    <row r="72" spans="12:12">
       <c r="L72" s="25"/>
     </row>
-    <row r="73" spans="1:12">
-      <c r="A73" s="7" t="s">
-        <v>62</v>
-      </c>
+    <row r="73" spans="12:12">
       <c r="L73" s="25"/>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="12:12">
       <c r="L74" s="25"/>
     </row>
-    <row r="75" spans="1:12">
-      <c r="A75" s="7" t="s">
-        <v>66</v>
-      </c>
+    <row r="75" spans="12:12">
       <c r="L75" s="25"/>
     </row>
-    <row r="76" spans="1:12">
-      <c r="A76" s="7" t="s">
-        <v>62</v>
-      </c>
+    <row r="76" spans="12:12">
       <c r="L76" s="25"/>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="12:12">
       <c r="L77" s="25"/>
     </row>
-    <row r="78" spans="1:12">
-      <c r="A78" s="7" t="s">
-        <v>67</v>
-      </c>
+    <row r="78" spans="12:12">
       <c r="L78" s="25"/>
     </row>
-    <row r="79" spans="1:12">
-      <c r="A79" s="7" t="s">
-        <v>68</v>
-      </c>
+    <row r="79" spans="12:12">
       <c r="L79" s="25"/>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="12:12">
       <c r="L80" s="25"/>
     </row>
-    <row r="81" spans="1:12">
-      <c r="A81" s="7" t="s">
-        <v>69</v>
-      </c>
+    <row r="81" spans="12:12">
       <c r="L81" s="25"/>
     </row>
-    <row r="82" spans="1:12">
-      <c r="A82" s="7" t="s">
-        <v>62</v>
-      </c>
+    <row r="82" spans="12:12">
       <c r="L82" s="25"/>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="12:12">
       <c r="L83" s="25"/>
     </row>
-    <row r="84" spans="1:12">
-      <c r="A84" s="7" t="s">
-        <v>70</v>
-      </c>
+    <row r="84" spans="12:12">
       <c r="L84" s="25"/>
     </row>
-    <row r="85" spans="1:12">
-      <c r="A85" s="7" t="s">
-        <v>71</v>
-      </c>
+    <row r="85" spans="12:12">
       <c r="L85" s="25"/>
     </row>
-    <row r="86" spans="1:12">
-      <c r="A86" s="7" t="s">
-        <v>72</v>
-      </c>
+    <row r="86" spans="12:12">
       <c r="L86" s="25"/>
     </row>
-    <row r="87" spans="1:12">
-      <c r="A87" s="7" t="s">
-        <v>62</v>
-      </c>
+    <row r="87" spans="12:12">
       <c r="L87" s="25"/>
     </row>
-    <row r="88" spans="1:12">
+    <row r="88" spans="12:12">
       <c r="L88" s="25"/>
     </row>
-    <row r="89" spans="1:12">
-      <c r="A89" s="7" t="s">
-        <v>73</v>
-      </c>
+    <row r="89" spans="12:12">
       <c r="L89" s="25"/>
     </row>
-    <row r="90" spans="1:12">
-      <c r="A90" s="7" t="s">
-        <v>74</v>
-      </c>
+    <row r="90" spans="12:12">
       <c r="L90" s="25"/>
     </row>
-    <row r="91" spans="1:12">
+    <row r="91" spans="12:12">
       <c r="L91" s="25"/>
     </row>
-    <row r="92" spans="1:12">
-      <c r="A92" s="7" t="s">
-        <v>75</v>
-      </c>
+    <row r="92" spans="12:12">
       <c r="L92" s="25"/>
     </row>
-    <row r="93" spans="1:12">
-      <c r="A93" s="7" t="s">
-        <v>76</v>
-      </c>
+    <row r="93" spans="12:12">
       <c r="L93" s="25"/>
     </row>
-    <row r="94" spans="1:12">
-      <c r="A94" s="7" t="s">
-        <v>77</v>
-      </c>
+    <row r="94" spans="12:12">
       <c r="L94" s="25"/>
     </row>
-    <row r="95" spans="1:12">
-      <c r="A95" s="7" t="s">
-        <v>78</v>
-      </c>
+    <row r="95" spans="12:12">
       <c r="L95" s="25"/>
     </row>
-    <row r="96" spans="1:12">
-      <c r="A96" s="7" t="s">
-        <v>79</v>
-      </c>
+    <row r="96" spans="12:12">
       <c r="L96" s="25"/>
     </row>
-    <row r="97" spans="1:12">
-      <c r="A97" s="7" t="s">
-        <v>80</v>
-      </c>
+    <row r="97" spans="12:12">
       <c r="L97" s="25"/>
     </row>
-    <row r="98" spans="1:12">
-      <c r="A98" s="7" t="s">
-        <v>81</v>
-      </c>
+    <row r="98" spans="12:12">
       <c r="L98" s="25"/>
     </row>
-    <row r="99" spans="1:12">
-      <c r="A99" s="7" t="s">
-        <v>82</v>
-      </c>
+    <row r="99" spans="12:12">
       <c r="L99" s="25"/>
     </row>
-    <row r="100" spans="1:12">
-      <c r="A100" s="7" t="s">
-        <v>83</v>
-      </c>
+    <row r="100" spans="12:12">
       <c r="L100" s="25"/>
     </row>
-    <row r="101" spans="1:12">
-      <c r="A101" s="7" t="s">
-        <v>84</v>
-      </c>
+    <row r="101" spans="12:12">
       <c r="L101" s="25"/>
     </row>
-    <row r="102" spans="1:12">
-      <c r="A102" s="7" t="s">
-        <v>85</v>
-      </c>
+    <row r="102" spans="12:12">
       <c r="L102" s="25"/>
     </row>
-    <row r="103" spans="1:12">
-      <c r="A103" s="7" t="s">
-        <v>86</v>
-      </c>
+    <row r="103" spans="12:12">
       <c r="L103" s="25"/>
     </row>
-    <row r="104" spans="1:12">
-      <c r="A104" s="7" t="s">
-        <v>62</v>
-      </c>
+    <row r="104" spans="12:12">
       <c r="L104" s="25"/>
     </row>
-    <row r="105" spans="1:12">
+    <row r="105" spans="12:12">
       <c r="L105" s="25"/>
     </row>
-    <row r="106" spans="1:12">
-      <c r="A106" s="7" t="s">
-        <v>87</v>
-      </c>
+    <row r="106" spans="12:12">
       <c r="L106" s="25"/>
     </row>
-    <row r="107" spans="1:12">
-      <c r="A107" s="7" t="s">
-        <v>88</v>
-      </c>
+    <row r="107" spans="12:12">
       <c r="L107" s="25"/>
     </row>
-    <row r="108" spans="1:12">
-      <c r="A108" s="7" t="s">
-        <v>89</v>
-      </c>
+    <row r="108" spans="12:12">
       <c r="L108" s="25"/>
     </row>
-    <row r="109" spans="1:12">
-      <c r="A109" s="7" t="s">
-        <v>68</v>
-      </c>
+    <row r="109" spans="12:12">
       <c r="L109" s="25"/>
     </row>
-    <row r="110" spans="1:12">
+    <row r="110" spans="12:12">
       <c r="L110" s="25"/>
     </row>
-    <row r="111" spans="1:12">
-      <c r="A111" s="7" t="s">
-        <v>90</v>
-      </c>
+    <row r="111" spans="12:12">
       <c r="L111" s="25"/>
     </row>
-    <row r="112" spans="1:12">
-      <c r="A112" s="7" t="s">
-        <v>91</v>
-      </c>
+    <row r="112" spans="12:12">
       <c r="L112" s="25"/>
     </row>
-    <row r="113" spans="1:12">
-      <c r="A113" s="7" t="s">
-        <v>92</v>
-      </c>
+    <row r="113" spans="12:12">
       <c r="L113" s="25"/>
     </row>
-    <row r="114" spans="1:12">
-      <c r="A114" s="7" t="s">
-        <v>93</v>
-      </c>
+    <row r="114" spans="12:12">
       <c r="L114" s="25"/>
     </row>
-    <row r="115" spans="1:12">
-      <c r="A115" s="7" t="s">
-        <v>94</v>
-      </c>
+    <row r="115" spans="12:12">
       <c r="L115" s="25"/>
     </row>
-    <row r="116" spans="1:12">
-      <c r="A116" s="7" t="s">
-        <v>95</v>
-      </c>
+    <row r="116" spans="12:12">
       <c r="L116" s="25"/>
     </row>
-    <row r="117" spans="1:12">
+    <row r="117" spans="12:12">
       <c r="L117" s="25"/>
     </row>
-    <row r="118" spans="1:12">
-      <c r="A118" s="7" t="s">
-        <v>96</v>
-      </c>
+    <row r="118" spans="12:12">
       <c r="L118" s="25"/>
     </row>
-    <row r="119" spans="1:12">
-      <c r="A119" s="7" t="s">
-        <v>97</v>
-      </c>
+    <row r="119" spans="12:12">
       <c r="L119" s="25"/>
     </row>
-    <row r="120" spans="1:12">
-      <c r="A120" s="7" t="s">
-        <v>98</v>
-      </c>
+    <row r="120" spans="12:12">
       <c r="L120" s="25"/>
     </row>
-    <row r="121" spans="1:12">
-      <c r="A121" s="7" t="s">
-        <v>99</v>
-      </c>
+    <row r="121" spans="12:12">
       <c r="L121" s="25"/>
     </row>
-    <row r="122" spans="1:12">
-      <c r="A122" s="7" t="s">
-        <v>100</v>
-      </c>
+    <row r="122" spans="12:12">
       <c r="L122" s="25"/>
     </row>
-    <row r="123" spans="1:12">
-      <c r="A123" s="7" t="s">
-        <v>101</v>
-      </c>
+    <row r="123" spans="12:12">
       <c r="L123" s="25"/>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" spans="12:12">
       <c r="L124" s="25"/>
     </row>
-    <row r="125" spans="1:12">
-      <c r="A125" s="7" t="s">
-        <v>102</v>
-      </c>
+    <row r="125" spans="12:12">
       <c r="L125" s="25"/>
     </row>
-    <row r="126" spans="1:12">
-      <c r="A126" s="7" t="s">
-        <v>103</v>
-      </c>
+    <row r="126" spans="12:12">
       <c r="L126" s="25"/>
     </row>
-    <row r="127" spans="1:12">
-      <c r="A127" s="7" t="s">
-        <v>104</v>
-      </c>
+    <row r="127" spans="12:12">
       <c r="L127" s="25"/>
     </row>
-    <row r="128" spans="1:12">
-      <c r="A128" s="7" t="s">
-        <v>105</v>
-      </c>
+    <row r="128" spans="12:12">
       <c r="L128" s="25"/>
     </row>
-    <row r="129" spans="1:12">
-      <c r="A129" s="7" t="s">
-        <v>106</v>
-      </c>
+    <row r="129" spans="12:12">
       <c r="L129" s="25"/>
     </row>
-    <row r="130" spans="1:12">
-      <c r="A130" s="7" t="s">
-        <v>107</v>
-      </c>
+    <row r="130" spans="12:12">
       <c r="L130" s="25"/>
     </row>
-    <row r="131" spans="1:12">
-      <c r="A131" s="7" t="s">
-        <v>108</v>
-      </c>
+    <row r="131" spans="12:12">
       <c r="L131" s="25"/>
     </row>
-    <row r="132" spans="1:12">
-      <c r="A132" s="7" t="s">
-        <v>109</v>
-      </c>
+    <row r="132" spans="12:12">
       <c r="L132" s="25"/>
     </row>
-    <row r="133" spans="1:12">
-      <c r="A133" s="7" t="s">
-        <v>110</v>
-      </c>
+    <row r="133" spans="12:12">
       <c r="L133" s="25"/>
     </row>
-    <row r="134" spans="1:12">
-      <c r="A134" s="7" t="s">
-        <v>111</v>
-      </c>
+    <row r="134" spans="12:12">
       <c r="L134" s="25"/>
     </row>
-    <row r="135" spans="1:12">
-      <c r="A135" s="7" t="s">
-        <v>112</v>
-      </c>
+    <row r="135" spans="12:12">
       <c r="L135" s="25"/>
     </row>
-    <row r="136" spans="1:12">
-      <c r="A136" s="7" t="s">
-        <v>113</v>
-      </c>
+    <row r="136" spans="12:12">
       <c r="L136" s="25"/>
     </row>
-    <row r="137" spans="1:12">
-      <c r="A137" s="7" t="s">
-        <v>114</v>
-      </c>
+    <row r="137" spans="12:12">
       <c r="L137" s="25"/>
     </row>
-    <row r="138" spans="1:12">
-      <c r="A138" s="7" t="s">
-        <v>115</v>
-      </c>
+    <row r="138" spans="12:12">
       <c r="L138" s="25"/>
     </row>
-    <row r="139" spans="1:12">
-      <c r="A139" s="7" t="s">
-        <v>116</v>
-      </c>
+    <row r="139" spans="12:12">
       <c r="L139" s="25"/>
     </row>
-    <row r="140" spans="1:12">
-      <c r="A140" s="7" t="s">
-        <v>117</v>
-      </c>
+    <row r="140" spans="12:12">
       <c r="L140" s="25"/>
     </row>
-    <row r="141" spans="1:12">
-      <c r="A141" s="7" t="s">
-        <v>118</v>
-      </c>
+    <row r="141" spans="12:12">
       <c r="L141" s="25"/>
     </row>
-    <row r="142" spans="1:12">
-      <c r="A142" s="7" t="s">
-        <v>119</v>
-      </c>
+    <row r="142" spans="12:12">
       <c r="L142" s="25"/>
     </row>
-    <row r="143" spans="1:12">
-      <c r="A143" s="7" t="s">
-        <v>120</v>
-      </c>
+    <row r="143" spans="12:12">
       <c r="L143" s="25"/>
     </row>
-    <row r="144" spans="1:12">
-      <c r="A144" s="7" t="s">
-        <v>121</v>
-      </c>
+    <row r="144" spans="12:12">
       <c r="L144" s="25"/>
     </row>
-    <row r="145" spans="1:12">
-      <c r="A145" s="7" t="s">
-        <v>122</v>
-      </c>
+    <row r="145" spans="12:12">
       <c r="L145" s="25"/>
     </row>
-    <row r="146" spans="1:12">
-      <c r="A146" s="7" t="s">
-        <v>123</v>
-      </c>
+    <row r="146" spans="12:12">
       <c r="L146" s="25"/>
     </row>
-    <row r="147" spans="1:12">
+    <row r="147" spans="12:12">
       <c r="L147" s="25"/>
     </row>
-    <row r="148" spans="1:12">
-      <c r="A148" s="7" t="s">
-        <v>124</v>
-      </c>
+    <row r="148" spans="12:12">
       <c r="L148" s="25"/>
     </row>
-    <row r="149" spans="1:12">
-      <c r="A149" s="7" t="s">
-        <v>125</v>
-      </c>
+    <row r="149" spans="12:12">
       <c r="L149" s="25"/>
     </row>
-    <row r="150" spans="1:12">
-      <c r="A150" s="7" t="s">
-        <v>126</v>
-      </c>
+    <row r="150" spans="12:12">
       <c r="L150" s="25"/>
     </row>
-    <row r="151" spans="1:12">
-      <c r="A151" s="7" t="s">
-        <v>127</v>
-      </c>
+    <row r="151" spans="12:12">
       <c r="L151" s="25"/>
     </row>
-    <row r="152" spans="1:12">
-      <c r="A152" s="7" t="s">
-        <v>128</v>
-      </c>
+    <row r="152" spans="12:12">
       <c r="L152" s="25"/>
     </row>
-    <row r="153" spans="1:12">
-      <c r="A153" s="7" t="s">
-        <v>129</v>
-      </c>
+    <row r="153" spans="12:12">
       <c r="L153" s="25"/>
     </row>
-    <row r="154" spans="1:12">
-      <c r="A154" s="7" t="s">
-        <v>130</v>
-      </c>
+    <row r="154" spans="12:12">
       <c r="L154" s="25"/>
     </row>
-    <row r="155" spans="1:12">
-      <c r="A155" s="7" t="s">
-        <v>131</v>
-      </c>
+    <row r="155" spans="12:12">
       <c r="L155" s="25"/>
     </row>
-    <row r="156" spans="1:12">
+    <row r="156" spans="12:12">
       <c r="L156" s="25"/>
     </row>
-    <row r="157" spans="1:12">
-      <c r="A157" s="7" t="s">
-        <v>132</v>
-      </c>
+    <row r="157" spans="12:12">
       <c r="L157" s="25"/>
     </row>
-    <row r="158" spans="1:12">
-      <c r="A158" s="7" t="s">
-        <v>133</v>
-      </c>
+    <row r="158" spans="12:12">
       <c r="L158" s="25"/>
     </row>
-    <row r="159" spans="1:12">
-      <c r="A159" s="7" t="s">
-        <v>62</v>
-      </c>
+    <row r="159" spans="12:12">
       <c r="L159" s="25"/>
     </row>
-    <row r="160" spans="1:12">
+    <row r="160" spans="12:12">
       <c r="L160" s="25"/>
     </row>
-    <row r="161" spans="1:12">
-      <c r="A161" s="7" t="s">
-        <v>134</v>
-      </c>
+    <row r="161" spans="12:12">
       <c r="L161" s="25"/>
     </row>
-    <row r="162" spans="1:12">
-      <c r="A162" s="7" t="s">
-        <v>135</v>
-      </c>
+    <row r="162" spans="12:12">
       <c r="L162" s="25"/>
     </row>
-    <row r="163" spans="1:12">
-      <c r="A163" s="7" t="s">
-        <v>136</v>
-      </c>
+    <row r="163" spans="12:12">
       <c r="L163" s="25"/>
     </row>
-    <row r="164" spans="1:12">
-      <c r="A164" s="7" t="s">
-        <v>137</v>
-      </c>
+    <row r="164" spans="12:12">
       <c r="L164" s="25"/>
     </row>
-    <row r="165" spans="1:12">
-      <c r="A165" s="7" t="s">
-        <v>138</v>
-      </c>
+    <row r="165" spans="12:12">
       <c r="L165" s="25"/>
     </row>
-    <row r="166" spans="1:12">
-      <c r="A166" s="7" t="s">
-        <v>139</v>
-      </c>
+    <row r="166" spans="12:12">
       <c r="L166" s="25"/>
     </row>
-    <row r="167" spans="1:12">
-      <c r="A167" s="7" t="s">
-        <v>140</v>
-      </c>
+    <row r="167" spans="12:12">
       <c r="L167" s="25"/>
     </row>
-    <row r="168" spans="1:12">
-      <c r="A168" s="7" t="s">
-        <v>62</v>
-      </c>
+    <row r="168" spans="12:12">
       <c r="L168" s="25"/>
     </row>
-    <row r="169" spans="1:12">
+    <row r="169" spans="12:12">
       <c r="L169" s="25"/>
     </row>
-    <row r="170" spans="1:12">
-      <c r="A170" s="7" t="s">
-        <v>141</v>
-      </c>
+    <row r="170" spans="12:12">
       <c r="L170" s="25"/>
     </row>
-    <row r="171" spans="1:12">
-      <c r="A171" s="7" t="s">
-        <v>142</v>
-      </c>
+    <row r="171" spans="12:12">
       <c r="L171" s="25"/>
     </row>
-    <row r="172" spans="1:12">
-      <c r="A172" s="7" t="s">
-        <v>143</v>
-      </c>
+    <row r="172" spans="12:12">
       <c r="L172" s="25"/>
     </row>
-    <row r="173" spans="1:12">
+    <row r="173" spans="12:12">
       <c r="L173" s="25"/>
     </row>
-    <row r="174" spans="1:12">
-      <c r="A174" s="7" t="s">
-        <v>144</v>
-      </c>
+    <row r="174" spans="12:12">
       <c r="L174" s="25"/>
     </row>
-    <row r="175" spans="1:12">
-      <c r="A175" s="7" t="s">
-        <v>145</v>
-      </c>
+    <row r="175" spans="12:12">
       <c r="L175" s="25"/>
     </row>
-    <row r="176" spans="1:12">
-      <c r="A176" s="7" t="s">
-        <v>146</v>
-      </c>
+    <row r="176" spans="12:12">
       <c r="L176" s="25"/>
     </row>
-    <row r="177" spans="1:12">
-      <c r="A177" s="7" t="s">
-        <v>147</v>
-      </c>
+    <row r="177" spans="12:12">
       <c r="L177" s="25"/>
     </row>
-    <row r="178" spans="1:12">
-      <c r="A178" s="7" t="s">
-        <v>148</v>
-      </c>
+    <row r="178" spans="12:12">
       <c r="L178" s="25"/>
     </row>
-    <row r="179" spans="1:12">
-      <c r="A179" s="7" t="s">
-        <v>143</v>
-      </c>
+    <row r="179" spans="12:12">
       <c r="L179" s="25"/>
     </row>
-    <row r="180" spans="1:12">
+    <row r="180" spans="12:12">
       <c r="L180" s="25"/>
     </row>
-    <row r="181" spans="1:12">
-      <c r="A181" s="7" t="s">
-        <v>149</v>
-      </c>
+    <row r="181" spans="12:12">
       <c r="L181" s="25"/>
     </row>
-    <row r="182" spans="1:12">
-      <c r="A182" s="7" t="s">
-        <v>150</v>
-      </c>
+    <row r="182" spans="12:12">
       <c r="L182" s="25"/>
     </row>
-    <row r="183" spans="1:12">
-      <c r="A183" s="7" t="s">
-        <v>151</v>
-      </c>
+    <row r="183" spans="12:12">
       <c r="L183" s="25"/>
     </row>
-    <row r="184" spans="1:12">
-      <c r="A184" s="7" t="s">
-        <v>62</v>
-      </c>
+    <row r="184" spans="12:12">
       <c r="L184" s="25"/>
     </row>
-    <row r="185" spans="1:12">
+    <row r="185" spans="12:12">
       <c r="L185" s="25"/>
     </row>
-    <row r="186" spans="1:12">
-      <c r="A186" s="7" t="s">
-        <v>152</v>
-      </c>
+    <row r="186" spans="12:12">
       <c r="L186" s="25"/>
     </row>
-    <row r="187" spans="1:12">
-      <c r="A187" s="7" t="s">
-        <v>153</v>
-      </c>
+    <row r="187" spans="12:12">
       <c r="L187" s="25"/>
     </row>
-    <row r="188" spans="1:12">
-      <c r="A188" s="7" t="s">
-        <v>154</v>
-      </c>
+    <row r="188" spans="12:12">
       <c r="L188" s="25"/>
     </row>
-    <row r="189" spans="1:12">
-      <c r="A189" s="7" t="s">
-        <v>62</v>
-      </c>
+    <row r="189" spans="12:12">
       <c r="L189" s="25"/>
     </row>
-    <row r="190" spans="1:12">
+    <row r="190" spans="12:12">
       <c r="L190" s="25"/>
     </row>
-    <row r="191" spans="1:12">
-      <c r="A191" s="7" t="s">
-        <v>155</v>
-      </c>
+    <row r="191" spans="12:12">
       <c r="L191" s="25"/>
     </row>
-    <row r="192" spans="1:12">
-      <c r="A192" s="7" t="s">
-        <v>156</v>
-      </c>
+    <row r="192" spans="12:12">
       <c r="L192" s="25"/>
     </row>
-    <row r="193" spans="1:12">
-      <c r="A193" s="7" t="s">
-        <v>157</v>
-      </c>
+    <row r="193" spans="12:12">
       <c r="L193" s="25"/>
     </row>
-    <row r="194" spans="1:12">
-      <c r="A194" s="7" t="s">
-        <v>158</v>
-      </c>
+    <row r="194" spans="12:12">
       <c r="L194" s="25"/>
     </row>
-    <row r="195" spans="1:12">
-      <c r="A195" s="7" t="s">
-        <v>159</v>
-      </c>
+    <row r="195" spans="12:12">
       <c r="L195" s="25"/>
     </row>
-    <row r="196" spans="1:12">
-      <c r="A196" s="7" t="s">
-        <v>160</v>
-      </c>
+    <row r="196" spans="12:12">
       <c r="L196" s="25"/>
     </row>
-    <row r="197" spans="1:12">
-      <c r="A197" s="7" t="s">
-        <v>161</v>
-      </c>
+    <row r="197" spans="12:12">
       <c r="L197" s="25"/>
     </row>
-    <row r="198" spans="1:12">
-      <c r="A198" s="7" t="s">
-        <v>162</v>
-      </c>
+    <row r="198" spans="12:12">
       <c r="L198" s="25"/>
     </row>
-    <row r="199" spans="1:12">
-      <c r="A199" s="7" t="s">
-        <v>163</v>
-      </c>
+    <row r="199" spans="12:12">
       <c r="L199" s="25"/>
     </row>
-    <row r="200" spans="1:12">
-      <c r="A200" s="7" t="s">
-        <v>164</v>
-      </c>
+    <row r="200" spans="12:12">
       <c r="L200" s="25"/>
     </row>
-    <row r="201" spans="1:12">
-      <c r="A201" s="7" t="s">
-        <v>165</v>
-      </c>
+    <row r="201" spans="12:12">
       <c r="L201" s="25"/>
     </row>
-    <row r="202" spans="1:12">
-      <c r="A202" s="7" t="s">
-        <v>166</v>
-      </c>
+    <row r="202" spans="12:12">
       <c r="L202" s="25"/>
     </row>
-    <row r="203" spans="1:12">
-      <c r="A203" s="7" t="s">
-        <v>167</v>
-      </c>
+    <row r="203" spans="12:12">
       <c r="L203" s="25"/>
     </row>
-    <row r="204" spans="1:12">
-      <c r="A204" s="7" t="s">
-        <v>168</v>
-      </c>
+    <row r="204" spans="12:12">
       <c r="L204" s="25"/>
     </row>
-    <row r="205" spans="1:12">
-      <c r="A205" s="7" t="s">
-        <v>169</v>
-      </c>
+    <row r="205" spans="12:12">
       <c r="L205" s="25"/>
     </row>
-    <row r="206" spans="1:12">
-      <c r="A206" s="7" t="s">
-        <v>170</v>
-      </c>
+    <row r="206" spans="12:12">
       <c r="L206" s="25"/>
     </row>
-    <row r="207" spans="1:12">
-      <c r="A207" s="7" t="s">
-        <v>171</v>
-      </c>
+    <row r="207" spans="12:12">
       <c r="L207" s="25"/>
     </row>
-    <row r="208" spans="1:12">
-      <c r="A208" s="7" t="s">
-        <v>172</v>
-      </c>
+    <row r="208" spans="12:12">
       <c r="L208" s="25"/>
     </row>
-    <row r="209" spans="1:12">
-      <c r="A209" s="7" t="s">
-        <v>173</v>
-      </c>
+    <row r="209" spans="12:12">
       <c r="L209" s="25"/>
     </row>
-    <row r="210" spans="1:12">
-      <c r="A210" s="7" t="s">
-        <v>174</v>
-      </c>
+    <row r="210" spans="12:12">
       <c r="L210" s="25"/>
     </row>
-    <row r="211" spans="1:12">
-      <c r="A211" s="7" t="s">
-        <v>62</v>
-      </c>
+    <row r="211" spans="12:12">
       <c r="L211" s="25"/>
     </row>
-    <row r="212" spans="1:12">
+    <row r="212" spans="12:12">
       <c r="L212" s="25"/>
     </row>
-    <row r="213" spans="1:12">
-      <c r="A213" s="7" t="s">
-        <v>175</v>
-      </c>
+    <row r="213" spans="12:12">
       <c r="L213" s="25"/>
     </row>
-    <row r="214" spans="1:12">
-      <c r="A214" s="7" t="s">
-        <v>176</v>
-      </c>
+    <row r="214" spans="12:12">
       <c r="L214" s="25"/>
     </row>
-    <row r="215" spans="1:12">
-      <c r="A215" s="7" t="s">
-        <v>177</v>
-      </c>
+    <row r="215" spans="12:12">
       <c r="L215" s="25"/>
     </row>
-    <row r="216" spans="1:12">
-      <c r="A216" s="7" t="s">
-        <v>178</v>
-      </c>
+    <row r="216" spans="12:12">
       <c r="L216" s="25"/>
     </row>
-    <row r="217" spans="1:12">
-      <c r="A217" s="7" t="s">
-        <v>179</v>
-      </c>
+    <row r="217" spans="12:12">
       <c r="L217" s="25"/>
     </row>
-    <row r="218" spans="1:12">
-      <c r="A218" s="7" t="s">
-        <v>180</v>
-      </c>
+    <row r="218" spans="12:12">
       <c r="L218" s="25"/>
     </row>
-    <row r="219" spans="1:12">
-      <c r="A219" s="7" t="s">
-        <v>181</v>
-      </c>
+    <row r="219" spans="12:12">
       <c r="L219" s="25"/>
     </row>
-    <row r="220" spans="1:12">
-      <c r="A220" s="7" t="s">
-        <v>182</v>
-      </c>
+    <row r="220" spans="12:12">
       <c r="L220" s="25"/>
     </row>
-    <row r="221" spans="1:12">
-      <c r="A221" s="7" t="s">
-        <v>183</v>
-      </c>
+    <row r="221" spans="12:12">
       <c r="L221" s="25"/>
     </row>
-    <row r="222" spans="1:12">
-      <c r="A222" s="7" t="s">
-        <v>184</v>
-      </c>
+    <row r="222" spans="12:12">
       <c r="L222" s="25"/>
     </row>
-    <row r="223" spans="1:12">
-      <c r="A223" s="7" t="s">
-        <v>185</v>
-      </c>
+    <row r="223" spans="12:12">
       <c r="L223" s="25"/>
     </row>
-    <row r="224" spans="1:12">
-      <c r="A224" s="7" t="s">
-        <v>186</v>
-      </c>
+    <row r="224" spans="12:12">
       <c r="L224" s="25"/>
     </row>
-    <row r="225" spans="1:12">
+    <row r="225" spans="12:12">
       <c r="L225" s="25"/>
     </row>
-    <row r="226" spans="1:12">
-      <c r="A226" s="7" t="s">
-        <v>187</v>
-      </c>
+    <row r="226" spans="12:12">
       <c r="L226" s="25"/>
     </row>
-    <row r="227" spans="1:12">
-      <c r="A227" s="7" t="s">
-        <v>188</v>
-      </c>
+    <row r="227" spans="12:12">
       <c r="L227" s="25"/>
     </row>
-    <row r="228" spans="1:12">
-      <c r="A228" s="7" t="s">
-        <v>189</v>
-      </c>
+    <row r="228" spans="12:12">
       <c r="L228" s="25"/>
     </row>
-    <row r="229" spans="1:12">
-      <c r="A229" s="7" t="s">
-        <v>190</v>
-      </c>
+    <row r="229" spans="12:12">
       <c r="L229" s="25"/>
     </row>
-    <row r="230" spans="1:12">
-      <c r="A230" s="7" t="s">
-        <v>191</v>
-      </c>
+    <row r="230" spans="12:12">
       <c r="L230" s="25"/>
     </row>
-    <row r="231" spans="1:12">
-      <c r="A231" s="7" t="s">
-        <v>192</v>
-      </c>
+    <row r="231" spans="12:12">
       <c r="L231" s="25"/>
     </row>
-    <row r="232" spans="1:12">
-      <c r="A232" s="7" t="s">
-        <v>193</v>
-      </c>
+    <row r="232" spans="12:12">
       <c r="L232" s="25"/>
     </row>
-    <row r="233" spans="1:12">
-      <c r="A233" s="7" t="s">
-        <v>194</v>
-      </c>
+    <row r="233" spans="12:12">
       <c r="L233" s="25"/>
     </row>
-    <row r="234" spans="1:12">
-      <c r="A234" s="7" t="s">
-        <v>195</v>
-      </c>
+    <row r="234" spans="12:12">
       <c r="L234" s="25"/>
     </row>
-    <row r="235" spans="1:12">
-      <c r="A235" s="7" t="s">
-        <v>196</v>
-      </c>
+    <row r="235" spans="12:12">
       <c r="L235" s="25"/>
     </row>
-    <row r="236" spans="1:12">
-      <c r="A236" s="7" t="s">
-        <v>197</v>
-      </c>
+    <row r="236" spans="12:12">
       <c r="L236" s="25"/>
     </row>
-    <row r="237" spans="1:12">
+    <row r="237" spans="12:12">
       <c r="L237" s="25"/>
     </row>
-    <row r="238" spans="1:12">
-      <c r="A238" s="7" t="s">
-        <v>198</v>
-      </c>
+    <row r="238" spans="12:12">
       <c r="L238" s="25"/>
     </row>
-    <row r="239" spans="1:12">
-      <c r="A239" s="7" t="s">
-        <v>199</v>
-      </c>
+    <row r="239" spans="12:12">
       <c r="L239" s="25"/>
     </row>
-    <row r="240" spans="1:12">
-      <c r="A240" s="7" t="s">
-        <v>200</v>
-      </c>
+    <row r="240" spans="12:12">
       <c r="L240" s="25"/>
     </row>
-    <row r="241" spans="1:12">
-      <c r="A241" s="7" t="s">
-        <v>201</v>
-      </c>
+    <row r="241" spans="12:12">
       <c r="L241" s="25"/>
     </row>
-    <row r="242" spans="1:12">
+    <row r="242" spans="12:12">
       <c r="L242" s="25"/>
     </row>
-    <row r="243" spans="1:12">
-      <c r="A243" s="7" t="s">
-        <v>202</v>
-      </c>
+    <row r="243" spans="12:12">
       <c r="L243" s="25"/>
     </row>
-    <row r="244" spans="1:12">
-      <c r="A244" s="7" t="s">
-        <v>71</v>
-      </c>
+    <row r="244" spans="12:12">
       <c r="L244" s="25"/>
     </row>
-    <row r="245" spans="1:12">
-      <c r="A245" s="7" t="s">
-        <v>72</v>
-      </c>
+    <row r="245" spans="12:12">
       <c r="L245" s="25"/>
     </row>
-    <row r="246" spans="1:12">
-      <c r="A246" s="7" t="s">
-        <v>68</v>
-      </c>
+    <row r="246" spans="12:12">
       <c r="L246" s="25"/>
     </row>
-    <row r="247" spans="1:12">
+    <row r="247" spans="12:12">
       <c r="L247" s="25"/>
     </row>
-    <row r="248" spans="1:12">
-      <c r="A248" s="7" t="s">
-        <v>203</v>
-      </c>
+    <row r="248" spans="12:12">
       <c r="L248" s="25"/>
     </row>
-    <row r="249" spans="1:12">
-      <c r="A249" s="7" t="s">
-        <v>204</v>
-      </c>
+    <row r="249" spans="12:12">
       <c r="L249" s="25"/>
     </row>
-    <row r="250" spans="1:12">
-      <c r="A250" s="7" t="s">
-        <v>205</v>
-      </c>
+    <row r="250" spans="12:12">
       <c r="L250" s="25"/>
     </row>
-    <row r="251" spans="1:12">
-      <c r="A251" s="7" t="s">
-        <v>62</v>
-      </c>
+    <row r="251" spans="12:12">
       <c r="L251" s="25"/>
     </row>
-    <row r="252" spans="1:12">
+    <row r="252" spans="12:12">
       <c r="L252" s="25"/>
     </row>
-    <row r="253" spans="1:12">
-      <c r="A253" s="7" t="s">
-        <v>206</v>
-      </c>
+    <row r="253" spans="12:12">
       <c r="L253" s="25"/>
     </row>
-    <row r="254" spans="1:12">
-      <c r="A254" s="7" t="s">
-        <v>207</v>
-      </c>
+    <row r="254" spans="12:12">
       <c r="L254" s="25"/>
     </row>
-    <row r="255" spans="1:12">
-      <c r="A255" s="7" t="s">
-        <v>208</v>
-      </c>
+    <row r="255" spans="12:12">
       <c r="L255" s="25"/>
     </row>
-    <row r="256" spans="1:12">
-      <c r="A256" s="7" t="s">
-        <v>209</v>
-      </c>
+    <row r="256" spans="12:12">
       <c r="L256" s="25"/>
     </row>
-    <row r="257" spans="1:12">
-      <c r="A257" s="7" t="s">
-        <v>210</v>
-      </c>
+    <row r="257" spans="12:12">
       <c r="L257" s="25"/>
     </row>
-    <row r="258" spans="1:12">
-      <c r="A258" s="7" t="s">
-        <v>62</v>
-      </c>
+    <row r="258" spans="12:12">
       <c r="L258" s="25"/>
     </row>
   </sheetData>

</xml_diff>